<commit_message>
i like this version
</commit_message>
<xml_diff>
--- a/restaurant_analytics/data.xlsx
+++ b/restaurant_analytics/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cardi\Documents\git-repo\swe_dev\restaurant_analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F83A19F-904F-4366-B434-4DEC476DA435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCF6207-B27B-418F-8488-77F1E8AD6C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5295" yWindow="-12300" windowWidth="21600" windowHeight="11295" xr2:uid="{284AE3AB-67B9-4275-829B-85B25FB0FD62}"/>
+    <workbookView xWindow="4275" yWindow="1890" windowWidth="21600" windowHeight="11295" xr2:uid="{284AE3AB-67B9-4275-829B-85B25FB0FD62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -474,11 +474,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECEB5D3-5A99-47D8-9F91-DA3E08A7A234}">
-  <dimension ref="A1:H354"/>
+  <dimension ref="A1:H365"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A344" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J356" sqref="J356"/>
+      <pane ySplit="1" topLeftCell="A350" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D363" sqref="D363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9690,6 +9690,265 @@
         <v>9.6</v>
       </c>
     </row>
+    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>2</v>
+      </c>
+      <c r="B355">
+        <v>354</v>
+      </c>
+      <c r="C355" s="3">
+        <v>45726</v>
+      </c>
+      <c r="D355">
+        <v>52</v>
+      </c>
+      <c r="E355">
+        <v>55.2</v>
+      </c>
+      <c r="F355">
+        <v>0</v>
+      </c>
+      <c r="G355">
+        <v>0</v>
+      </c>
+      <c r="H355">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A356">
+        <v>3</v>
+      </c>
+      <c r="B356">
+        <v>355</v>
+      </c>
+      <c r="C356" s="3">
+        <v>45727</v>
+      </c>
+      <c r="D356">
+        <v>95</v>
+      </c>
+      <c r="E356">
+        <v>45.1</v>
+      </c>
+      <c r="F356">
+        <v>0</v>
+      </c>
+      <c r="G356">
+        <v>0</v>
+      </c>
+      <c r="H356">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A357">
+        <v>4</v>
+      </c>
+      <c r="B357">
+        <v>356</v>
+      </c>
+      <c r="C357" s="3">
+        <v>45728</v>
+      </c>
+      <c r="E357">
+        <v>43.9</v>
+      </c>
+      <c r="F357">
+        <v>0</v>
+      </c>
+      <c r="G357">
+        <v>0</v>
+      </c>
+      <c r="H357">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <v>5</v>
+      </c>
+      <c r="B358">
+        <v>357</v>
+      </c>
+      <c r="C358" s="3">
+        <v>45729</v>
+      </c>
+      <c r="E358">
+        <v>49.6</v>
+      </c>
+      <c r="F358">
+        <v>0</v>
+      </c>
+      <c r="G358">
+        <v>0</v>
+      </c>
+      <c r="H358">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A359">
+        <v>6</v>
+      </c>
+      <c r="B359">
+        <v>358</v>
+      </c>
+      <c r="C359" s="3">
+        <v>45730</v>
+      </c>
+      <c r="E359">
+        <v>58.5</v>
+      </c>
+      <c r="F359">
+        <v>0.15</v>
+      </c>
+      <c r="G359">
+        <v>0</v>
+      </c>
+      <c r="H359">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <v>7</v>
+      </c>
+      <c r="B360">
+        <v>359</v>
+      </c>
+      <c r="C360" s="3">
+        <v>45731</v>
+      </c>
+      <c r="E360">
+        <v>54.1</v>
+      </c>
+      <c r="F360">
+        <v>0.25</v>
+      </c>
+      <c r="G360">
+        <v>0</v>
+      </c>
+      <c r="H360">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>1</v>
+      </c>
+      <c r="B361">
+        <v>360</v>
+      </c>
+      <c r="C361" s="3">
+        <v>45732</v>
+      </c>
+      <c r="E361">
+        <v>40.5</v>
+      </c>
+      <c r="F361">
+        <v>0.05</v>
+      </c>
+      <c r="G361">
+        <v>1</v>
+      </c>
+      <c r="H361">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A362">
+        <v>2</v>
+      </c>
+      <c r="B362">
+        <v>361</v>
+      </c>
+      <c r="C362" s="3">
+        <v>45733</v>
+      </c>
+      <c r="E362">
+        <v>39.4</v>
+      </c>
+      <c r="F362">
+        <v>0</v>
+      </c>
+      <c r="G362">
+        <v>0</v>
+      </c>
+      <c r="H362">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>3</v>
+      </c>
+      <c r="B363">
+        <v>362</v>
+      </c>
+      <c r="C363" s="3">
+        <v>45734</v>
+      </c>
+      <c r="E363">
+        <v>42.3</v>
+      </c>
+      <c r="F363">
+        <v>0</v>
+      </c>
+      <c r="G363">
+        <v>0</v>
+      </c>
+      <c r="H363">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A364">
+        <v>4</v>
+      </c>
+      <c r="B364">
+        <v>363</v>
+      </c>
+      <c r="C364" s="3">
+        <v>45735</v>
+      </c>
+      <c r="E364">
+        <v>43.7</v>
+      </c>
+      <c r="F364">
+        <v>0</v>
+      </c>
+      <c r="G364">
+        <v>0</v>
+      </c>
+      <c r="H364">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A365">
+        <v>5</v>
+      </c>
+      <c r="B365">
+        <v>364</v>
+      </c>
+      <c r="C365" s="3">
+        <v>45736</v>
+      </c>
+      <c r="E365">
+        <v>44.8</v>
+      </c>
+      <c r="F365">
+        <v>0.8</v>
+      </c>
+      <c r="G365">
+        <v>0.1</v>
+      </c>
+      <c r="H365">
+        <v>11.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding graphs and finetuning model
</commit_message>
<xml_diff>
--- a/restaurant_analytics/data.xlsx
+++ b/restaurant_analytics/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cardi\Documents\git-repo\swe_dev\restaurant_analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCF6207-B27B-418F-8488-77F1E8AD6C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0447226-61AE-4963-AA35-5063CB226D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="1890" windowWidth="21600" windowHeight="11295" xr2:uid="{284AE3AB-67B9-4275-829B-85B25FB0FD62}"/>
+    <workbookView xWindow="7185" yWindow="210" windowWidth="21600" windowHeight="11295" xr2:uid="{284AE3AB-67B9-4275-829B-85B25FB0FD62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -474,11 +474,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECEB5D3-5A99-47D8-9F91-DA3E08A7A234}">
-  <dimension ref="A1:H365"/>
+  <dimension ref="A1:H367"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A350" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D363" sqref="D363"/>
+      <pane ySplit="1" topLeftCell="A353" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G364" sqref="G364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9701,10 +9701,10 @@
         <v>45726</v>
       </c>
       <c r="D355">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E355">
-        <v>55.2</v>
+        <v>52.5</v>
       </c>
       <c r="F355">
         <v>0</v>
@@ -9727,10 +9727,10 @@
         <v>45727</v>
       </c>
       <c r="D356">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E356">
-        <v>45.1</v>
+        <v>45</v>
       </c>
       <c r="F356">
         <v>0</v>
@@ -9739,7 +9739,7 @@
         <v>0</v>
       </c>
       <c r="H356">
-        <v>12</v>
+        <v>16.100000000000001</v>
       </c>
     </row>
     <row r="357" spans="1:8" x14ac:dyDescent="0.25">
@@ -9752,8 +9752,11 @@
       <c r="C357" s="3">
         <v>45728</v>
       </c>
+      <c r="D357">
+        <v>37</v>
+      </c>
       <c r="E357">
-        <v>43.9</v>
+        <v>42.6</v>
       </c>
       <c r="F357">
         <v>0</v>
@@ -9775,8 +9778,11 @@
       <c r="C358" s="3">
         <v>45729</v>
       </c>
+      <c r="D358">
+        <v>41</v>
+      </c>
       <c r="E358">
-        <v>49.6</v>
+        <v>46.4</v>
       </c>
       <c r="F358">
         <v>0</v>
@@ -9799,16 +9805,16 @@
         <v>45730</v>
       </c>
       <c r="E359">
-        <v>58.5</v>
+        <v>59.4</v>
       </c>
       <c r="F359">
-        <v>0.15</v>
+        <v>0.5</v>
       </c>
       <c r="G359">
         <v>0</v>
       </c>
       <c r="H359">
-        <v>12.6</v>
+        <v>13.2</v>
       </c>
     </row>
     <row r="360" spans="1:8" x14ac:dyDescent="0.25">
@@ -9822,16 +9828,16 @@
         <v>45731</v>
       </c>
       <c r="E360">
-        <v>54.1</v>
+        <v>57.9</v>
       </c>
       <c r="F360">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="G360">
         <v>0</v>
       </c>
       <c r="H360">
-        <v>18</v>
+        <v>18.2</v>
       </c>
     </row>
     <row r="361" spans="1:8" x14ac:dyDescent="0.25">
@@ -9845,16 +9851,16 @@
         <v>45732</v>
       </c>
       <c r="E361">
-        <v>40.5</v>
+        <v>39.9</v>
       </c>
       <c r="F361">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="G361">
         <v>1</v>
       </c>
       <c r="H361">
-        <v>12.6</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="362" spans="1:8" x14ac:dyDescent="0.25">
@@ -9868,7 +9874,7 @@
         <v>45733</v>
       </c>
       <c r="E362">
-        <v>39.4</v>
+        <v>43.7</v>
       </c>
       <c r="F362">
         <v>0</v>
@@ -9877,7 +9883,7 @@
         <v>0</v>
       </c>
       <c r="H362">
-        <v>10.5</v>
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="363" spans="1:8" x14ac:dyDescent="0.25">
@@ -9891,7 +9897,7 @@
         <v>45734</v>
       </c>
       <c r="E363">
-        <v>42.3</v>
+        <v>52.5</v>
       </c>
       <c r="F363">
         <v>0</v>
@@ -9900,7 +9906,7 @@
         <v>0</v>
       </c>
       <c r="H363">
-        <v>11.1</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="364" spans="1:8" x14ac:dyDescent="0.25">
@@ -9914,16 +9920,16 @@
         <v>45735</v>
       </c>
       <c r="E364">
-        <v>43.7</v>
+        <v>50.9</v>
       </c>
       <c r="F364">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G364">
         <v>0</v>
       </c>
       <c r="H364">
-        <v>11</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="365" spans="1:8" x14ac:dyDescent="0.25">
@@ -9937,16 +9943,62 @@
         <v>45736</v>
       </c>
       <c r="E365">
-        <v>44.8</v>
+        <v>42.4</v>
       </c>
       <c r="F365">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="G365">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="H365">
-        <v>11.2</v>
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A366">
+        <v>6</v>
+      </c>
+      <c r="B366">
+        <v>365</v>
+      </c>
+      <c r="C366" s="3">
+        <v>45737</v>
+      </c>
+      <c r="E366">
+        <v>40.5</v>
+      </c>
+      <c r="F366">
+        <v>0</v>
+      </c>
+      <c r="G366">
+        <v>0</v>
+      </c>
+      <c r="H366">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A367">
+        <v>7</v>
+      </c>
+      <c r="B367">
+        <v>366</v>
+      </c>
+      <c r="C367" s="3">
+        <v>45738</v>
+      </c>
+      <c r="E367">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="F367">
+        <v>0</v>
+      </c>
+      <c r="G367">
+        <v>0</v>
+      </c>
+      <c r="H367">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feeling good about predictions
</commit_message>
<xml_diff>
--- a/restaurant_analytics/data.xlsx
+++ b/restaurant_analytics/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cardi\Documents\git-repo\swe_dev\restaurant_analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C81F20-4770-40BA-9A80-C3D28E422CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98476756-B077-43A6-AF3D-DBBB9A7EEA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="2250" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6450" yWindow="1545" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,20 @@
   <definedNames>
     <definedName name="day">Sheet1!$A$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -128,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -160,9 +173,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -473,8 +483,8 @@
   <dimension ref="A1:H409"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A360" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D364" sqref="D364"/>
+      <pane ySplit="1" topLeftCell="A388" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H394" sqref="H394"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9808,7 +9818,7 @@
         <v>116</v>
       </c>
       <c r="E359" s="10">
-        <v>64.5</v>
+        <v>59.7</v>
       </c>
       <c r="F359" s="10">
         <v>0</v>
@@ -9817,7 +9827,7 @@
         <v>0</v>
       </c>
       <c r="H359" s="10">
-        <v>12.4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="360" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9834,7 +9844,7 @@
         <v>180</v>
       </c>
       <c r="E360" s="10">
-        <v>57</v>
+        <v>54.9</v>
       </c>
       <c r="F360" s="10">
         <v>0.53</v>
@@ -9843,7 +9853,7 @@
         <v>0</v>
       </c>
       <c r="H360" s="10">
-        <v>13</v>
+        <v>18.600000000000001</v>
       </c>
     </row>
     <row r="361" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9860,7 +9870,7 @@
         <v>110</v>
       </c>
       <c r="E361" s="10">
-        <v>33.200000000000003</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="F361" s="10">
         <v>0.22</v>
@@ -9869,7 +9879,7 @@
         <v>1</v>
       </c>
       <c r="H361" s="10">
-        <v>12.8</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="362" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9886,7 +9896,7 @@
         <v>4</v>
       </c>
       <c r="E362" s="10">
-        <v>44.5</v>
+        <v>40.5</v>
       </c>
       <c r="F362" s="10">
         <v>0.5</v>
@@ -9895,7 +9905,7 @@
         <v>0</v>
       </c>
       <c r="H362" s="10">
-        <v>10.199999999999999</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="363" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9909,10 +9919,10 @@
         <v>45734</v>
       </c>
       <c r="D363" s="4">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E363" s="10">
-        <v>54.7</v>
+        <v>45.9</v>
       </c>
       <c r="F363" s="10">
         <v>0</v>
@@ -9921,7 +9931,7 @@
         <v>0</v>
       </c>
       <c r="H363" s="10">
-        <v>12.6</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="364" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9935,10 +9945,10 @@
         <v>45735</v>
       </c>
       <c r="D364" s="4">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E364" s="10">
-        <v>42.7</v>
+        <v>47.1</v>
       </c>
       <c r="F364" s="10">
         <v>0.8</v>
@@ -9947,7 +9957,7 @@
         <v>1</v>
       </c>
       <c r="H364" s="10">
-        <v>12.9</v>
+        <v>11.6</v>
       </c>
     </row>
     <row r="365" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9961,10 +9971,10 @@
         <v>45736</v>
       </c>
       <c r="D365" s="4">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="E365" s="10">
-        <v>42.4</v>
+        <v>44.4</v>
       </c>
       <c r="F365" s="10">
         <v>0.5</v>
@@ -9973,7 +9983,7 @@
         <v>1.9</v>
       </c>
       <c r="H365" s="10">
-        <v>13.4</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="366" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9987,10 +9997,10 @@
         <v>45737</v>
       </c>
       <c r="D366" s="4">
-        <v>154</v>
+        <v>104</v>
       </c>
       <c r="E366" s="10">
-        <v>40.5</v>
+        <v>46.67</v>
       </c>
       <c r="F366" s="10">
         <v>0</v>
@@ -10013,10 +10023,10 @@
         <v>45738</v>
       </c>
       <c r="D367" s="4">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="E367" s="10">
-        <v>40.799999999999997</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="F367" s="10">
         <v>0</v>
@@ -10025,7 +10035,7 @@
         <v>0</v>
       </c>
       <c r="H367" s="10">
-        <v>11</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="368" spans="1:8" x14ac:dyDescent="0.25">
@@ -10039,19 +10049,19 @@
         <v>45739</v>
       </c>
       <c r="D368" s="8">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E368" s="9">
-        <v>41.5</v>
-      </c>
-      <c r="F368" s="13">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="F368" s="12">
         <v>0.06</v>
       </c>
       <c r="G368" s="10">
         <v>0</v>
       </c>
       <c r="H368" s="9">
-        <v>10</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="369" spans="1:8" x14ac:dyDescent="0.25">
@@ -10065,7 +10075,7 @@
         <v>45740</v>
       </c>
       <c r="D369" s="8">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="E369" s="9">
         <v>34.75</v>
@@ -10091,7 +10101,7 @@
         <v>45741</v>
       </c>
       <c r="D370" s="8">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E370" s="9">
         <v>36.5</v>
@@ -10117,7 +10127,7 @@
         <v>45742</v>
       </c>
       <c r="D371" s="8">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E371" s="9">
         <v>38.5</v>
@@ -10143,7 +10153,7 @@
         <v>45743</v>
       </c>
       <c r="D372" s="8">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E372" s="9">
         <v>41.75</v>
@@ -10169,7 +10179,7 @@
         <v>45744</v>
       </c>
       <c r="D373" s="8">
-        <v>76</v>
+        <v>128</v>
       </c>
       <c r="E373" s="9">
         <v>47.5</v>
@@ -10195,7 +10205,7 @@
         <v>45745</v>
       </c>
       <c r="D374" s="8">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="E374" s="9">
         <v>53</v>
@@ -10221,7 +10231,7 @@
         <v>45746</v>
       </c>
       <c r="D375" s="8">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E375" s="9">
         <v>49.25</v>
@@ -10247,7 +10257,7 @@
         <v>45747</v>
       </c>
       <c r="D376" s="8">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E376" s="9">
         <v>44.5</v>
@@ -10299,7 +10309,7 @@
         <v>45749</v>
       </c>
       <c r="D378" s="8">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="E378" s="9">
         <v>48</v>
@@ -10351,7 +10361,7 @@
         <v>45751</v>
       </c>
       <c r="D380" s="8">
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="E380" s="9">
         <v>44.5</v>
@@ -10377,7 +10387,7 @@
         <v>45752</v>
       </c>
       <c r="D381" s="8">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="E381" s="9">
         <v>45.5</v>
@@ -10403,7 +10413,7 @@
         <v>45753</v>
       </c>
       <c r="D382" s="8">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E382" s="9">
         <v>44.5</v>
@@ -10429,12 +10439,12 @@
         <v>45754</v>
       </c>
       <c r="D383" s="8">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E383" s="9">
         <v>45</v>
       </c>
-      <c r="F383" s="13">
+      <c r="F383" s="12">
         <v>0.64</v>
       </c>
       <c r="G383" s="10">
@@ -10455,12 +10465,12 @@
         <v>45755</v>
       </c>
       <c r="D384" s="8">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E384" s="9">
         <v>46.5</v>
       </c>
-      <c r="F384" s="13">
+      <c r="F384" s="12">
         <v>0</v>
       </c>
       <c r="G384" s="10">
@@ -10481,12 +10491,12 @@
         <v>45756</v>
       </c>
       <c r="D385" s="8">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E385" s="9">
         <v>45.5</v>
       </c>
-      <c r="F385" s="13">
+      <c r="F385" s="12">
         <v>0.41</v>
       </c>
       <c r="G385" s="10">
@@ -10507,12 +10517,12 @@
         <v>45757</v>
       </c>
       <c r="D386" s="8">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E386" s="9">
         <v>41.5</v>
       </c>
-      <c r="F386" s="13">
+      <c r="F386" s="12">
         <v>0.12</v>
       </c>
       <c r="G386" s="10">
@@ -10533,12 +10543,12 @@
         <v>45758</v>
       </c>
       <c r="D387" s="8">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="E387" s="9">
         <v>40.5</v>
       </c>
-      <c r="F387" s="13">
+      <c r="F387" s="12">
         <v>0</v>
       </c>
       <c r="G387" s="10">
@@ -10559,12 +10569,12 @@
         <v>45759</v>
       </c>
       <c r="D388" s="8">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="E388" s="9">
         <v>40</v>
       </c>
-      <c r="F388" s="13">
+      <c r="F388" s="12">
         <v>0</v>
       </c>
       <c r="G388" s="10">
@@ -10585,12 +10595,12 @@
         <v>45760</v>
       </c>
       <c r="D389" s="8">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E389" s="9">
         <v>43</v>
       </c>
-      <c r="F389" s="13">
+      <c r="F389" s="12">
         <v>0</v>
       </c>
       <c r="G389" s="10">
@@ -10616,7 +10626,7 @@
       <c r="E390" s="9">
         <v>48</v>
       </c>
-      <c r="F390" s="13">
+      <c r="F390" s="12">
         <v>0</v>
       </c>
       <c r="G390" s="10">
@@ -10637,12 +10647,12 @@
         <v>45762</v>
       </c>
       <c r="D391" s="8">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E391" s="9">
         <v>42.5</v>
       </c>
-      <c r="F391" s="13">
+      <c r="F391" s="12">
         <v>0</v>
       </c>
       <c r="G391" s="10">
@@ -10663,12 +10673,12 @@
         <v>45763</v>
       </c>
       <c r="D392" s="8">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="E392" s="9">
         <v>49</v>
       </c>
-      <c r="F392" s="13">
+      <c r="F392" s="12">
         <v>0.19</v>
       </c>
       <c r="G392" s="10">
@@ -10689,12 +10699,12 @@
         <v>45764</v>
       </c>
       <c r="D393" s="8">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="E393" s="9">
         <v>55</v>
       </c>
-      <c r="F393" s="13">
+      <c r="F393" s="12">
         <v>0</v>
       </c>
       <c r="G393" s="10">
@@ -10720,7 +10730,7 @@
       <c r="E394" s="9">
         <v>56</v>
       </c>
-      <c r="F394" s="13">
+      <c r="F394" s="12">
         <v>0</v>
       </c>
       <c r="G394" s="10">
@@ -10741,12 +10751,12 @@
         <v>45766</v>
       </c>
       <c r="D395" s="8">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="E395" s="9">
         <v>55</v>
       </c>
-      <c r="F395" s="13">
+      <c r="F395" s="12">
         <v>0</v>
       </c>
       <c r="G395" s="10">
@@ -10772,7 +10782,7 @@
       <c r="E396" s="9">
         <v>54</v>
       </c>
-      <c r="F396" s="13">
+      <c r="F396" s="12">
         <v>0</v>
       </c>
       <c r="G396" s="10">
@@ -10798,7 +10808,7 @@
       <c r="E397" s="9">
         <v>50.5</v>
       </c>
-      <c r="F397" s="13">
+      <c r="F397" s="12">
         <v>0.36</v>
       </c>
       <c r="G397" s="10">
@@ -10824,7 +10834,7 @@
       <c r="E398" s="9">
         <v>51</v>
       </c>
-      <c r="F398" s="13">
+      <c r="F398" s="12">
         <v>0.52</v>
       </c>
       <c r="G398" s="10">
@@ -10850,7 +10860,7 @@
       <c r="E399" s="9">
         <v>53</v>
       </c>
-      <c r="F399" s="13">
+      <c r="F399" s="12">
         <v>0</v>
       </c>
       <c r="G399" s="10">
@@ -10871,12 +10881,12 @@
         <v>45771</v>
       </c>
       <c r="D400" s="8">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E400" s="9">
         <v>53</v>
       </c>
-      <c r="F400" s="13">
+      <c r="F400" s="12">
         <v>0.24</v>
       </c>
       <c r="G400" s="10">
@@ -10902,7 +10912,7 @@
       <c r="E401" s="9">
         <v>54.5</v>
       </c>
-      <c r="F401" s="13">
+      <c r="F401" s="12">
         <v>0.03</v>
       </c>
       <c r="G401" s="10">
@@ -10928,7 +10938,7 @@
       <c r="E402" s="9">
         <v>53.5</v>
       </c>
-      <c r="F402" s="13">
+      <c r="F402" s="12">
         <v>0</v>
       </c>
       <c r="G402" s="10">
@@ -10949,12 +10959,12 @@
         <v>45774</v>
       </c>
       <c r="D403" s="8">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E403" s="9">
         <v>48.5</v>
       </c>
-      <c r="F403" s="13">
+      <c r="F403" s="12">
         <v>0</v>
       </c>
       <c r="G403" s="10">
@@ -10975,12 +10985,12 @@
         <v>45775</v>
       </c>
       <c r="D404" s="8">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E404" s="9">
         <v>54.5</v>
       </c>
-      <c r="F404" s="13">
+      <c r="F404" s="12">
         <v>0.59</v>
       </c>
       <c r="G404" s="10">
@@ -11001,12 +11011,12 @@
         <v>45776</v>
       </c>
       <c r="D405" s="8">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E405" s="9">
         <v>50.5</v>
       </c>
-      <c r="F405" s="13">
+      <c r="F405" s="12">
         <v>0</v>
       </c>
       <c r="G405" s="10">
@@ -11027,7 +11037,7 @@
         <v>45777</v>
       </c>
       <c r="D406" s="8">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E406" s="12">
         <v>52</v>
@@ -11053,7 +11063,7 @@
         <v>45778</v>
       </c>
       <c r="D407" s="8">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E407" s="12">
         <v>55</v>

</xml_diff>

<commit_message>
note: 32x4 giving 30%+ results
</commit_message>
<xml_diff>
--- a/restaurant_analytics/data.xlsx
+++ b/restaurant_analytics/data.xlsx
@@ -10470,7 +10470,7 @@
         <v>45756</v>
       </c>
       <c r="D385" s="5">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="E385" s="7">
         <v>39.7</v>
@@ -10496,10 +10496,10 @@
         <v>45757</v>
       </c>
       <c r="D386" s="5">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E386" s="7">
-        <v>42.4</v>
+        <v>39.9</v>
       </c>
       <c r="F386" s="7">
         <v>0.12</v>
@@ -10508,7 +10508,7 @@
         <v>0</v>
       </c>
       <c r="H386" s="7">
-        <v>8.5</v>
+        <v>10.3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="387" customHeight="1" ht="18.75">
@@ -10522,10 +10522,10 @@
         <v>45758</v>
       </c>
       <c r="D387" s="5">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="E387" s="7">
-        <v>44.2</v>
+        <v>44.1</v>
       </c>
       <c r="F387" s="7">
         <v>0</v>
@@ -10534,7 +10534,7 @@
         <v>0</v>
       </c>
       <c r="H387" s="7">
-        <v>8.9</v>
+        <v>8.3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="388" customHeight="1" ht="18.75">
@@ -10548,10 +10548,10 @@
         <v>45759</v>
       </c>
       <c r="D388" s="5">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E388" s="7">
-        <v>48.2</v>
+        <v>50</v>
       </c>
       <c r="F388" s="7">
         <v>0</v>
@@ -10560,7 +10560,7 @@
         <v>0</v>
       </c>
       <c r="H388" s="7">
-        <v>6.6</v>
+        <v>6.2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="389" customHeight="1" ht="18.75">
@@ -10574,10 +10574,10 @@
         <v>45760</v>
       </c>
       <c r="D389" s="5">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E389" s="7">
-        <v>55.2</v>
+        <v>57.7</v>
       </c>
       <c r="F389" s="7">
         <v>0</v>
@@ -10586,7 +10586,7 @@
         <v>0</v>
       </c>
       <c r="H389" s="7">
-        <v>11.4</v>
+        <v>12.8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="390" customHeight="1" ht="18.75">
@@ -10600,10 +10600,10 @@
         <v>45761</v>
       </c>
       <c r="D390" s="5">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="E390" s="7">
-        <v>56.3</v>
+        <v>56.8</v>
       </c>
       <c r="F390" s="7">
         <v>0</v>
@@ -10612,7 +10612,7 @@
         <v>0</v>
       </c>
       <c r="H390" s="7">
-        <v>12.2</v>
+        <v>14.7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="391" customHeight="1" ht="18.75">
@@ -10626,19 +10626,19 @@
         <v>45762</v>
       </c>
       <c r="D391" s="5">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E391" s="7">
-        <v>48.9</v>
+        <v>46.8</v>
       </c>
       <c r="F391" s="7">
-        <v>0</v>
+        <v>0.016</v>
       </c>
       <c r="G391" s="7">
         <v>0</v>
       </c>
       <c r="H391" s="7">
-        <v>11.7</v>
+        <v>16.7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="392" customHeight="1" ht="18.75">
@@ -10652,19 +10652,19 @@
         <v>45763</v>
       </c>
       <c r="D392" s="5">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E392" s="7">
-        <v>48.9</v>
+        <v>45.5</v>
       </c>
       <c r="F392" s="7">
-        <v>0.19</v>
+        <v>0</v>
       </c>
       <c r="G392" s="7">
         <v>0</v>
       </c>
       <c r="H392" s="7">
-        <v>10.4</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="393" customHeight="1" ht="18.75">
@@ -10678,10 +10678,10 @@
         <v>45764</v>
       </c>
       <c r="D393" s="5">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E393" s="7">
-        <v>50.9</v>
+        <v>54.7</v>
       </c>
       <c r="F393" s="7">
         <v>0</v>
@@ -10690,7 +10690,7 @@
         <v>0</v>
       </c>
       <c r="H393" s="7">
-        <v>10.7</v>
+        <v>12.6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="394" customHeight="1" ht="18.75">
@@ -10707,16 +10707,16 @@
         <v>141</v>
       </c>
       <c r="E394" s="7">
-        <v>56</v>
+        <v>57.6</v>
       </c>
       <c r="F394" s="7">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="G394" s="7">
         <v>0</v>
       </c>
       <c r="H394" s="7">
-        <v>13</v>
+        <v>10.4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="395" customHeight="1" ht="18.75">
@@ -10733,16 +10733,16 @@
         <v>162</v>
       </c>
       <c r="E395" s="7">
-        <v>55</v>
+        <v>50.9</v>
       </c>
       <c r="F395" s="7">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="G395" s="7">
         <v>0</v>
       </c>
       <c r="H395" s="7">
-        <v>10</v>
+        <v>9.8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="396" customHeight="1" ht="18.75">
@@ -10756,19 +10756,19 @@
         <v>45767</v>
       </c>
       <c r="D396" s="5">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E396" s="7">
-        <v>54</v>
+        <v>52.3</v>
       </c>
       <c r="F396" s="7">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G396" s="7">
         <v>0</v>
       </c>
       <c r="H396" s="7">
-        <v>10</v>
+        <v>11.7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="397" customHeight="1" ht="18.75">
@@ -10782,19 +10782,19 @@
         <v>45768</v>
       </c>
       <c r="D397" s="5">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E397" s="7">
-        <v>50.5</v>
+        <v>56.3</v>
       </c>
       <c r="F397" s="7">
-        <v>0.36</v>
+        <v>0.4</v>
       </c>
       <c r="G397" s="7">
         <v>0</v>
       </c>
       <c r="H397" s="7">
-        <v>10</v>
+        <v>10.6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="398" customHeight="1" ht="18.75">
@@ -10808,19 +10808,19 @@
         <v>45769</v>
       </c>
       <c r="D398" s="5">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E398" s="7">
-        <v>51</v>
+        <v>56.5</v>
       </c>
       <c r="F398" s="7">
-        <v>0.52</v>
+        <v>0</v>
       </c>
       <c r="G398" s="7">
         <v>0</v>
       </c>
       <c r="H398" s="7">
-        <v>12</v>
+        <v>0.2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="399" customHeight="1" ht="18.75">
@@ -10834,10 +10834,10 @@
         <v>45770</v>
       </c>
       <c r="D399" s="5">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="E399" s="7">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F399" s="7">
         <v>0</v>
@@ -10860,13 +10860,13 @@
         <v>45771</v>
       </c>
       <c r="D400" s="5">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="E400" s="7">
         <v>53</v>
       </c>
       <c r="F400" s="7">
-        <v>0.24</v>
+        <v>0.05</v>
       </c>
       <c r="G400" s="7">
         <v>0</v>
@@ -10938,7 +10938,7 @@
         <v>45774</v>
       </c>
       <c r="D403" s="5">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E403" s="7">
         <v>48.5</v>
@@ -10964,7 +10964,7 @@
         <v>45775</v>
       </c>
       <c r="D404" s="5">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E404" s="7">
         <v>54.5</v>
@@ -11016,7 +11016,7 @@
         <v>45777</v>
       </c>
       <c r="D406" s="5">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E406" s="7">
         <v>52</v>
@@ -11042,7 +11042,7 @@
         <v>45778</v>
       </c>
       <c r="D407" s="5">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E407" s="7">
         <v>55</v>

</xml_diff>

<commit_message>
trying to lower test loss
</commit_message>
<xml_diff>
--- a/restaurant_analytics/data.xlsx
+++ b/restaurant_analytics/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cardi\Documents\git-repo\swe_dev\restaurant_analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2B7CBB-EEF1-4FD2-BD01-BAAEA880C2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B0C512-787F-41EA-A0EC-44FB1068178B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30180" yWindow="405" windowWidth="25755" windowHeight="14130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -156,7 +156,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +175,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -237,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -279,6 +285,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,8 +596,8 @@
   <dimension ref="A1:K467"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A420" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D438" sqref="D438"/>
+      <pane ySplit="1" topLeftCell="A433" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L448" sqref="L448"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12349,7 +12358,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="433" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A433" s="6">
         <v>3</v>
       </c>
@@ -12360,7 +12369,7 @@
         <v>45804</v>
       </c>
       <c r="D433">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E433" s="10">
         <v>61.3</v>
@@ -12374,9 +12383,9 @@
       <c r="H433" s="10">
         <v>8.9</v>
       </c>
-      <c r="I433"/>
-    </row>
-    <row r="434" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K433" s="15"/>
+    </row>
+    <row r="434" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A434" s="6">
         <v>4</v>
       </c>
@@ -12387,7 +12396,7 @@
         <v>45805</v>
       </c>
       <c r="D434" s="14">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E434" s="10">
         <v>63.9</v>
@@ -12402,8 +12411,9 @@
         <v>8.9</v>
       </c>
       <c r="I434"/>
-    </row>
-    <row r="435" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K434" s="15"/>
+    </row>
+    <row r="435" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A435" s="6">
         <v>5</v>
       </c>
@@ -12414,7 +12424,7 @@
         <v>45806</v>
       </c>
       <c r="D435">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E435" s="10">
         <v>64.8</v>
@@ -12429,8 +12439,9 @@
         <v>9.1</v>
       </c>
       <c r="I435"/>
-    </row>
-    <row r="436" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K435" s="15"/>
+    </row>
+    <row r="436" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A436" s="6">
         <v>6</v>
       </c>
@@ -12441,7 +12452,7 @@
         <v>45807</v>
       </c>
       <c r="D436">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="E436" s="10">
         <v>58</v>
@@ -12456,8 +12467,9 @@
         <v>9</v>
       </c>
       <c r="I436"/>
-    </row>
-    <row r="437" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K436" s="15"/>
+    </row>
+    <row r="437" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A437" s="6">
         <v>7</v>
       </c>
@@ -12468,7 +12480,7 @@
         <v>45808</v>
       </c>
       <c r="D437">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="E437" s="10">
         <v>60</v>
@@ -12483,8 +12495,9 @@
         <v>4</v>
       </c>
       <c r="I437"/>
-    </row>
-    <row r="438" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K437" s="15"/>
+    </row>
+    <row r="438" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A438" s="9">
         <v>1</v>
       </c>
@@ -12495,7 +12508,7 @@
         <v>45809</v>
       </c>
       <c r="D438">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E438" s="10">
         <v>62</v>
@@ -12510,8 +12523,9 @@
         <v>6</v>
       </c>
       <c r="I438"/>
-    </row>
-    <row r="439" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K438" s="15"/>
+    </row>
+    <row r="439" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A439" s="6">
         <v>2</v>
       </c>
@@ -12522,7 +12536,7 @@
         <v>45810</v>
       </c>
       <c r="D439">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E439" s="10">
         <v>63</v>
@@ -12537,8 +12551,9 @@
         <v>10</v>
       </c>
       <c r="I439"/>
-    </row>
-    <row r="440" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K439" s="15"/>
+    </row>
+    <row r="440" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A440" s="6">
         <v>3</v>
       </c>
@@ -12549,7 +12564,7 @@
         <v>45811</v>
       </c>
       <c r="D440">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E440" s="10">
         <v>63</v>
@@ -12564,8 +12579,9 @@
         <v>7</v>
       </c>
       <c r="I440"/>
-    </row>
-    <row r="441" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K440" s="15"/>
+    </row>
+    <row r="441" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A441" s="6">
         <v>4</v>
       </c>
@@ -12576,7 +12592,7 @@
         <v>45812</v>
       </c>
       <c r="D441">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E441" s="10">
         <v>64</v>
@@ -12591,8 +12607,9 @@
         <v>7</v>
       </c>
       <c r="I441"/>
-    </row>
-    <row r="442" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K441" s="15"/>
+    </row>
+    <row r="442" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A442" s="6">
         <v>5</v>
       </c>
@@ -12603,7 +12620,7 @@
         <v>45813</v>
       </c>
       <c r="D442">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E442" s="10">
         <v>63</v>
@@ -12618,8 +12635,9 @@
         <v>9</v>
       </c>
       <c r="I442"/>
-    </row>
-    <row r="443" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K442" s="15"/>
+    </row>
+    <row r="443" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A443" s="6">
         <v>6</v>
       </c>
@@ -12630,7 +12648,7 @@
         <v>45814</v>
       </c>
       <c r="D443">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="E443" s="10">
         <v>61</v>
@@ -12645,8 +12663,9 @@
         <v>6</v>
       </c>
       <c r="I443"/>
-    </row>
-    <row r="444" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K443" s="15"/>
+    </row>
+    <row r="444" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A444" s="6">
         <v>7</v>
       </c>
@@ -12657,7 +12676,7 @@
         <v>45815</v>
       </c>
       <c r="D444">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="E444" s="10">
         <v>60</v>
@@ -12672,8 +12691,9 @@
         <v>5</v>
       </c>
       <c r="I444"/>
-    </row>
-    <row r="445" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K444" s="15"/>
+    </row>
+    <row r="445" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A445" s="9">
         <v>1</v>
       </c>
@@ -12684,7 +12704,7 @@
         <v>45816</v>
       </c>
       <c r="D445">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E445" s="10">
         <v>61</v>
@@ -12699,8 +12719,9 @@
         <v>7</v>
       </c>
       <c r="I445"/>
-    </row>
-    <row r="446" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K445" s="15"/>
+    </row>
+    <row r="446" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A446" s="6">
         <v>2</v>
       </c>
@@ -12711,7 +12732,7 @@
         <v>45817</v>
       </c>
       <c r="D446">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E446" s="10">
         <v>61</v>
@@ -12726,8 +12747,9 @@
         <v>7</v>
       </c>
       <c r="I446"/>
-    </row>
-    <row r="447" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K446" s="15"/>
+    </row>
+    <row r="447" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A447" s="6">
         <v>3</v>
       </c>
@@ -12738,7 +12760,7 @@
         <v>45818</v>
       </c>
       <c r="D447">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E447" s="10">
         <v>61</v>
@@ -12753,8 +12775,9 @@
         <v>2</v>
       </c>
       <c r="I447"/>
-    </row>
-    <row r="448" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K447" s="15"/>
+    </row>
+    <row r="448" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A448" s="6">
         <v>4</v>
       </c>
@@ -12765,7 +12788,7 @@
         <v>45819</v>
       </c>
       <c r="D448">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E448" s="10">
         <v>63</v>
@@ -12780,8 +12803,9 @@
         <v>6</v>
       </c>
       <c r="I448"/>
-    </row>
-    <row r="449" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K448" s="15"/>
+    </row>
+    <row r="449" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A449" s="6">
         <v>5</v>
       </c>
@@ -12792,7 +12816,7 @@
         <v>45820</v>
       </c>
       <c r="D449">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E449" s="10">
         <v>69</v>
@@ -12807,8 +12831,9 @@
         <v>8</v>
       </c>
       <c r="I449"/>
-    </row>
-    <row r="450" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K449" s="15"/>
+    </row>
+    <row r="450" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A450" s="6">
         <v>6</v>
       </c>
@@ -12819,7 +12844,7 @@
         <v>45821</v>
       </c>
       <c r="D450">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E450" s="10">
         <v>66</v>
@@ -12834,8 +12859,9 @@
         <v>6</v>
       </c>
       <c r="I450"/>
-    </row>
-    <row r="451" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K450" s="15"/>
+    </row>
+    <row r="451" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A451" s="6">
         <v>7</v>
       </c>
@@ -12846,7 +12872,7 @@
         <v>45822</v>
       </c>
       <c r="D451">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E451" s="10">
         <v>69</v>
@@ -12861,8 +12887,9 @@
         <v>4</v>
       </c>
       <c r="I451"/>
-    </row>
-    <row r="452" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K451" s="15"/>
+    </row>
+    <row r="452" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A452" s="9">
         <v>1</v>
       </c>
@@ -12873,7 +12900,7 @@
         <v>45823</v>
       </c>
       <c r="D452">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="E452" s="10">
         <v>67</v>
@@ -12890,8 +12917,9 @@
       <c r="I452" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="453" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K452" s="15"/>
+    </row>
+    <row r="453" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A453" s="6">
         <v>2</v>
       </c>
@@ -12902,7 +12930,7 @@
         <v>45824</v>
       </c>
       <c r="D453">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E453" s="10">
         <v>63</v>
@@ -12917,8 +12945,9 @@
         <v>6</v>
       </c>
       <c r="I453"/>
-    </row>
-    <row r="454" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K453" s="15"/>
+    </row>
+    <row r="454" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A454" s="6">
         <v>3</v>
       </c>
@@ -12929,7 +12958,7 @@
         <v>45825</v>
       </c>
       <c r="D454">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E454" s="10">
         <v>70</v>
@@ -12944,8 +12973,9 @@
         <v>8</v>
       </c>
       <c r="I454"/>
-    </row>
-    <row r="455" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K454" s="15"/>
+    </row>
+    <row r="455" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A455" s="6">
         <v>4</v>
       </c>
@@ -12956,7 +12986,7 @@
         <v>45826</v>
       </c>
       <c r="D455">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E455" s="10">
         <v>70</v>
@@ -12971,8 +13001,9 @@
         <v>14</v>
       </c>
       <c r="I455"/>
-    </row>
-    <row r="456" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K455" s="15"/>
+    </row>
+    <row r="456" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A456" s="6">
         <v>5</v>
       </c>
@@ -12983,7 +13014,7 @@
         <v>45827</v>
       </c>
       <c r="D456">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E456" s="10">
         <v>70</v>
@@ -12998,8 +13029,9 @@
         <v>9</v>
       </c>
       <c r="I456"/>
-    </row>
-    <row r="457" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K456" s="15"/>
+    </row>
+    <row r="457" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A457" s="6">
         <v>6</v>
       </c>
@@ -13010,7 +13042,7 @@
         <v>45828</v>
       </c>
       <c r="D457">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E457" s="10">
         <v>69</v>
@@ -13025,8 +13057,9 @@
         <v>8</v>
       </c>
       <c r="I457"/>
-    </row>
-    <row r="458" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K457" s="15"/>
+    </row>
+    <row r="458" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A458" s="6">
         <v>7</v>
       </c>
@@ -13037,7 +13070,7 @@
         <v>45829</v>
       </c>
       <c r="D458">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E458" s="10">
         <v>71</v>
@@ -13052,8 +13085,9 @@
         <v>5</v>
       </c>
       <c r="I458"/>
-    </row>
-    <row r="459" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K458" s="15"/>
+    </row>
+    <row r="459" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A459" s="9">
         <v>1</v>
       </c>
@@ -13064,7 +13098,7 @@
         <v>45830</v>
       </c>
       <c r="D459">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E459" s="10">
         <v>74</v>
@@ -13079,8 +13113,9 @@
         <v>3</v>
       </c>
       <c r="I459"/>
-    </row>
-    <row r="460" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K459" s="15"/>
+    </row>
+    <row r="460" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A460" s="6">
         <v>2</v>
       </c>
@@ -13091,7 +13126,7 @@
         <v>45831</v>
       </c>
       <c r="D460">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="E460" s="10">
         <v>75</v>
@@ -13106,8 +13141,9 @@
         <v>2</v>
       </c>
       <c r="I460"/>
-    </row>
-    <row r="461" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K460" s="15"/>
+    </row>
+    <row r="461" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A461" s="6">
         <v>3</v>
       </c>
@@ -13118,7 +13154,7 @@
         <v>45832</v>
       </c>
       <c r="D461">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E461" s="10">
         <v>75</v>
@@ -13133,8 +13169,9 @@
         <v>8</v>
       </c>
       <c r="I461"/>
-    </row>
-    <row r="462" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K461" s="15"/>
+    </row>
+    <row r="462" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A462" s="6">
         <v>4</v>
       </c>
@@ -13145,7 +13182,7 @@
         <v>45833</v>
       </c>
       <c r="D462">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E462" s="10">
         <v>76</v>
@@ -13160,8 +13197,9 @@
         <v>8</v>
       </c>
       <c r="I462"/>
-    </row>
-    <row r="463" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K462" s="15"/>
+    </row>
+    <row r="463" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A463" s="6">
         <v>5</v>
       </c>
@@ -13172,7 +13210,7 @@
         <v>45834</v>
       </c>
       <c r="D463">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="E463" s="10">
         <v>76</v>
@@ -13187,8 +13225,9 @@
         <v>4</v>
       </c>
       <c r="I463"/>
-    </row>
-    <row r="464" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K463" s="15"/>
+    </row>
+    <row r="464" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A464" s="6">
         <v>6</v>
       </c>
@@ -13199,7 +13238,7 @@
         <v>45835</v>
       </c>
       <c r="D464">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="E464" s="10">
         <v>75</v>
@@ -13214,8 +13253,9 @@
         <v>6</v>
       </c>
       <c r="I464"/>
-    </row>
-    <row r="465" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K464" s="15"/>
+    </row>
+    <row r="465" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A465" s="6">
         <v>7</v>
       </c>
@@ -13226,7 +13266,7 @@
         <v>45836</v>
       </c>
       <c r="D465">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E465" s="10">
         <v>71</v>
@@ -13241,8 +13281,9 @@
         <v>8</v>
       </c>
       <c r="I465"/>
-    </row>
-    <row r="466" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K465" s="15"/>
+    </row>
+    <row r="466" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A466" s="9">
         <v>1</v>
       </c>
@@ -13253,7 +13294,7 @@
         <v>45837</v>
       </c>
       <c r="D466">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E466" s="10">
         <v>71</v>
@@ -13268,8 +13309,9 @@
         <v>6</v>
       </c>
       <c r="I466"/>
-    </row>
-    <row r="467" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K466" s="15"/>
+    </row>
+    <row r="467" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A467" s="9">
         <v>2</v>
       </c>
@@ -13280,7 +13322,7 @@
         <v>45838</v>
       </c>
       <c r="D467">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E467" s="10">
         <v>73</v>
@@ -13295,6 +13337,7 @@
         <v>5</v>
       </c>
       <c r="I467"/>
+      <c r="K467" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added iteration and averages of averages
</commit_message>
<xml_diff>
--- a/restaurant_analytics/data.xlsx
+++ b/restaurant_analytics/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cardi\Documents\git-repo\swe_dev\restaurant_analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90D9041-5FF1-4486-AC3A-B40E454BB6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45322F00-9CB5-4B88-9436-BF5DE32AF6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -398,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -477,6 +477,14 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -850,9 +858,9 @@
   </sheetPr>
   <dimension ref="A1:K513"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A445" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q454" sqref="Q454"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A472" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J479" sqref="J478:J479"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13169,7 +13177,7 @@
         <v>52</v>
       </c>
       <c r="E466" s="9">
-        <v>81.099999999999994</v>
+        <v>81.7</v>
       </c>
       <c r="F466" s="9">
         <v>3.1E-2</v>
@@ -13197,10 +13205,10 @@
         <v>122</v>
       </c>
       <c r="E467" s="9">
-        <v>79.7</v>
+        <v>81.900000000000006</v>
       </c>
       <c r="F467" s="9">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="G467" s="9">
         <v>0</v>
@@ -13225,7 +13233,7 @@
         <v>82</v>
       </c>
       <c r="E468" s="11">
-        <v>79.5</v>
+        <v>79.7</v>
       </c>
       <c r="F468" s="11">
         <v>0</v>
@@ -13251,10 +13259,10 @@
         <v>69</v>
       </c>
       <c r="E469" s="11">
-        <v>81.099999999999994</v>
+        <v>80.599999999999994</v>
       </c>
       <c r="F469" s="11">
-        <v>4.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="G469" s="9">
         <v>0</v>
@@ -13277,7 +13285,7 @@
         <v>137</v>
       </c>
       <c r="E470" s="11">
-        <v>83.1</v>
+        <v>80.8</v>
       </c>
       <c r="F470" s="11">
         <v>0</v>
@@ -13306,7 +13314,7 @@
         <v>82</v>
       </c>
       <c r="F471" s="11">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="G471" s="9">
         <v>0</v>
@@ -13335,7 +13343,7 @@
         <v>85.5</v>
       </c>
       <c r="F472" s="11">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G472" s="9">
         <v>0</v>
@@ -13355,22 +13363,19 @@
         <v>45844</v>
       </c>
       <c r="D473" s="16">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="E473" s="11">
-        <v>76.5</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="F473" s="11">
-        <v>0.28299999999999997</v>
+        <v>0</v>
       </c>
       <c r="G473" s="11">
         <v>0</v>
       </c>
       <c r="H473" s="11">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="J473" s="11">
-        <v>10.14</v>
+        <v>11.6</v>
       </c>
     </row>
     <row r="474" spans="1:11" x14ac:dyDescent="0.25">
@@ -13384,22 +13389,19 @@
         <v>45845</v>
       </c>
       <c r="D474" s="16">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="E474" s="11">
-        <v>72.5</v>
+        <v>72.900000000000006</v>
       </c>
       <c r="F474" s="11">
-        <v>0</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G474" s="11">
         <v>0</v>
       </c>
       <c r="H474" s="11">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="J474" s="11">
-        <v>18.559999999999999</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="475" spans="1:11" x14ac:dyDescent="0.25">
@@ -13413,10 +13415,10 @@
         <v>45846</v>
       </c>
       <c r="D475" s="16">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E475" s="11">
-        <v>75.2</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="F475" s="11">
         <v>0</v>
@@ -13425,10 +13427,7 @@
         <v>0</v>
       </c>
       <c r="H475" s="11">
-        <v>5.2</v>
-      </c>
-      <c r="J475" s="11">
-        <v>6.53</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="476" spans="1:11" x14ac:dyDescent="0.25">
@@ -13442,22 +13441,19 @@
         <v>45847</v>
       </c>
       <c r="D476" s="16">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="E476" s="11">
-        <v>76.099999999999994</v>
+        <v>75.7</v>
       </c>
       <c r="F476" s="11">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="G476" s="11">
         <v>0</v>
       </c>
       <c r="H476" s="11">
-        <v>6.1</v>
-      </c>
-      <c r="J476" s="11">
-        <v>17.97</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="477" spans="1:11" x14ac:dyDescent="0.25">
@@ -13471,10 +13467,10 @@
         <v>45848</v>
       </c>
       <c r="D477" s="16">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="E477" s="11">
-        <v>75.599999999999994</v>
+        <v>74.3</v>
       </c>
       <c r="F477" s="11">
         <v>0</v>
@@ -13484,9 +13480,6 @@
       </c>
       <c r="H477" s="11">
         <v>6.6</v>
-      </c>
-      <c r="J477" s="11">
-        <v>22.01</v>
       </c>
     </row>
     <row r="478" spans="1:11" x14ac:dyDescent="0.25">
@@ -13499,23 +13492,20 @@
       <c r="C478" s="8">
         <v>45849</v>
       </c>
-      <c r="D478" s="16">
-        <v>190</v>
+      <c r="D478">
+        <v>146</v>
       </c>
       <c r="E478" s="11">
-        <v>77.5</v>
+        <v>77.900000000000006</v>
       </c>
       <c r="F478" s="11">
-        <v>0.28000000000000003</v>
+        <v>1.29</v>
       </c>
       <c r="G478" s="11">
         <v>0</v>
       </c>
       <c r="H478" s="11">
-        <v>6.4</v>
-      </c>
-      <c r="J478" s="11">
-        <v>20.309999999999999</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="479" spans="1:11" x14ac:dyDescent="0.25">
@@ -13528,23 +13518,20 @@
       <c r="C479" s="8">
         <v>45850</v>
       </c>
-      <c r="D479" s="16">
-        <v>163</v>
+      <c r="D479">
+        <v>178</v>
       </c>
       <c r="E479" s="11">
-        <v>76.8</v>
+        <v>77.7</v>
       </c>
       <c r="F479" s="11">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="G479" s="11">
         <v>0</v>
       </c>
       <c r="H479" s="11">
-        <v>8.5</v>
-      </c>
-      <c r="J479" s="11">
-        <v>3.51</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="480" spans="1:11" x14ac:dyDescent="0.25">
@@ -13557,11 +13544,11 @@
       <c r="C480" s="8">
         <v>45851</v>
       </c>
-      <c r="D480" s="16">
-        <v>70</v>
+      <c r="D480">
+        <v>83</v>
       </c>
       <c r="E480" s="11">
-        <v>75.7</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="F480" s="11">
         <v>0</v>
@@ -13570,10 +13557,10 @@
         <v>0</v>
       </c>
       <c r="H480" s="11">
-        <v>8</v>
+        <v>8.6</v>
       </c>
       <c r="J480" s="11">
-        <v>11.91</v>
+        <v>5.58</v>
       </c>
     </row>
     <row r="481" spans="1:10" x14ac:dyDescent="0.25">
@@ -13586,11 +13573,11 @@
       <c r="C481" s="8">
         <v>45852</v>
       </c>
-      <c r="D481" s="16">
-        <v>76</v>
+      <c r="D481">
+        <v>80</v>
       </c>
       <c r="E481" s="11">
-        <v>75.7</v>
+        <v>77.2</v>
       </c>
       <c r="F481" s="11">
         <v>0</v>
@@ -13599,10 +13586,10 @@
         <v>0</v>
       </c>
       <c r="H481" s="11">
-        <v>7.7</v>
+        <v>7.5</v>
       </c>
       <c r="J481" s="11">
-        <v>10.48</v>
+        <v>5.59</v>
       </c>
     </row>
     <row r="482" spans="1:10" x14ac:dyDescent="0.25">
@@ -13615,11 +13602,11 @@
       <c r="C482" s="8">
         <v>45853</v>
       </c>
-      <c r="D482" s="16">
-        <v>77</v>
+      <c r="D482">
+        <v>82</v>
       </c>
       <c r="E482" s="11">
-        <v>76.099999999999994</v>
+        <v>76.8</v>
       </c>
       <c r="F482" s="11">
         <v>0</v>
@@ -13628,10 +13615,10 @@
         <v>0</v>
       </c>
       <c r="H482" s="11">
-        <v>8.4</v>
+        <v>7.8</v>
       </c>
       <c r="J482" s="11">
-        <v>8.67</v>
+        <v>4.3099999999999996</v>
       </c>
     </row>
     <row r="483" spans="1:10" x14ac:dyDescent="0.25">
@@ -13644,23 +13631,23 @@
       <c r="C483" s="8">
         <v>45854</v>
       </c>
-      <c r="D483" s="16">
+      <c r="D483">
         <v>79</v>
       </c>
       <c r="E483" s="11">
-        <v>75.5</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="F483" s="11">
-        <v>0.13</v>
+        <v>0.65</v>
       </c>
       <c r="G483" s="11">
         <v>0</v>
       </c>
       <c r="H483" s="11">
-        <v>6</v>
+        <v>8.1</v>
       </c>
       <c r="J483" s="11">
-        <v>17.309999999999999</v>
+        <v>8.27</v>
       </c>
     </row>
     <row r="484" spans="1:10" x14ac:dyDescent="0.25">
@@ -13673,23 +13660,23 @@
       <c r="C484" s="8">
         <v>45855</v>
       </c>
-      <c r="D484" s="16">
-        <v>82</v>
+      <c r="D484">
+        <v>107</v>
       </c>
       <c r="E484" s="11">
-        <v>74.5</v>
+        <v>75.2</v>
       </c>
       <c r="F484" s="11">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="G484" s="11">
         <v>0</v>
       </c>
       <c r="H484" s="11">
-        <v>5</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="J484" s="11">
-        <v>13.07</v>
+        <v>9.44</v>
       </c>
     </row>
     <row r="485" spans="1:10" x14ac:dyDescent="0.25">
@@ -13702,8 +13689,8 @@
       <c r="C485" s="8">
         <v>45856</v>
       </c>
-      <c r="D485" s="16">
-        <v>132</v>
+      <c r="D485">
+        <v>133</v>
       </c>
       <c r="E485" s="11">
         <v>76</v>
@@ -13718,7 +13705,7 @@
         <v>13</v>
       </c>
       <c r="J485" s="11">
-        <v>7.64</v>
+        <v>14.37</v>
       </c>
     </row>
     <row r="486" spans="1:10" x14ac:dyDescent="0.25">
@@ -13731,14 +13718,14 @@
       <c r="C486" s="8">
         <v>45857</v>
       </c>
-      <c r="D486" s="16">
-        <v>170</v>
+      <c r="D486">
+        <v>169</v>
       </c>
       <c r="E486" s="11">
         <v>75</v>
       </c>
       <c r="F486" s="11">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G486" s="11">
         <v>0</v>
@@ -13747,7 +13734,7 @@
         <v>7</v>
       </c>
       <c r="J486" s="11">
-        <v>4.12</v>
+        <v>5.68</v>
       </c>
     </row>
     <row r="487" spans="1:10" x14ac:dyDescent="0.25">
@@ -13760,8 +13747,8 @@
       <c r="C487" s="8">
         <v>45858</v>
       </c>
-      <c r="D487" s="16">
-        <v>48</v>
+      <c r="D487">
+        <v>47</v>
       </c>
       <c r="E487" s="11">
         <v>69.5</v>
@@ -13776,7 +13763,7 @@
         <v>6</v>
       </c>
       <c r="J487" s="11">
-        <v>4.87</v>
+        <v>8.01</v>
       </c>
     </row>
     <row r="488" spans="1:10" x14ac:dyDescent="0.25">
@@ -13789,8 +13776,8 @@
       <c r="C488" s="8">
         <v>45859</v>
       </c>
-      <c r="D488" s="16">
-        <v>62</v>
+      <c r="D488">
+        <v>61</v>
       </c>
       <c r="E488" s="11">
         <v>69</v>
@@ -13805,7 +13792,7 @@
         <v>4</v>
       </c>
       <c r="J488" s="11">
-        <v>4.46</v>
+        <v>5.28</v>
       </c>
     </row>
     <row r="489" spans="1:10" x14ac:dyDescent="0.25">
@@ -13818,8 +13805,8 @@
       <c r="C489" s="8">
         <v>45860</v>
       </c>
-      <c r="D489" s="16">
-        <v>91</v>
+      <c r="D489">
+        <v>87</v>
       </c>
       <c r="E489" s="11">
         <v>74.5</v>
@@ -13834,7 +13821,7 @@
         <v>7</v>
       </c>
       <c r="J489" s="11">
-        <v>12.34</v>
+        <v>12.95</v>
       </c>
     </row>
     <row r="490" spans="1:10" x14ac:dyDescent="0.25">
@@ -13847,8 +13834,8 @@
       <c r="C490" s="8">
         <v>45861</v>
       </c>
-      <c r="D490" s="16">
-        <v>57</v>
+      <c r="D490">
+        <v>62</v>
       </c>
       <c r="E490" s="11">
         <v>76</v>
@@ -13863,7 +13850,7 @@
         <v>5</v>
       </c>
       <c r="J490" s="11">
-        <v>11.36</v>
+        <v>3.44</v>
       </c>
     </row>
     <row r="491" spans="1:10" x14ac:dyDescent="0.25">
@@ -13876,8 +13863,8 @@
       <c r="C491" s="8">
         <v>45862</v>
       </c>
-      <c r="D491" s="16">
-        <v>78</v>
+      <c r="D491">
+        <v>74</v>
       </c>
       <c r="E491" s="11">
         <v>73</v>
@@ -13892,7 +13879,7 @@
         <v>5</v>
       </c>
       <c r="J491" s="11">
-        <v>8.2200000000000006</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="492" spans="1:10" x14ac:dyDescent="0.25">
@@ -13905,8 +13892,8 @@
       <c r="C492" s="8">
         <v>45863</v>
       </c>
-      <c r="D492" s="16">
-        <v>188</v>
+      <c r="D492">
+        <v>184</v>
       </c>
       <c r="E492" s="11">
         <v>72</v>
@@ -13921,7 +13908,7 @@
         <v>7</v>
       </c>
       <c r="J492" s="11">
-        <v>10.050000000000001</v>
+        <v>14.57</v>
       </c>
     </row>
     <row r="493" spans="1:10" x14ac:dyDescent="0.25">
@@ -13934,8 +13921,8 @@
       <c r="C493" s="8">
         <v>45864</v>
       </c>
-      <c r="D493" s="16">
-        <v>188</v>
+      <c r="D493">
+        <v>183</v>
       </c>
       <c r="E493" s="11">
         <v>70</v>
@@ -13950,7 +13937,7 @@
         <v>5</v>
       </c>
       <c r="J493" s="11">
-        <v>3.65</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="494" spans="1:10" x14ac:dyDescent="0.25">
@@ -13963,8 +13950,8 @@
       <c r="C494" s="8">
         <v>45865</v>
       </c>
-      <c r="D494" s="16">
-        <v>68</v>
+      <c r="D494">
+        <v>61</v>
       </c>
       <c r="E494" s="11">
         <v>73.5</v>
@@ -13979,7 +13966,7 @@
         <v>9</v>
       </c>
       <c r="J494" s="11">
-        <v>11.37</v>
+        <v>4.74</v>
       </c>
     </row>
     <row r="495" spans="1:10" x14ac:dyDescent="0.25">
@@ -13992,8 +13979,8 @@
       <c r="C495" s="8">
         <v>45866</v>
       </c>
-      <c r="D495" s="16">
-        <v>64</v>
+      <c r="D495">
+        <v>61</v>
       </c>
       <c r="E495" s="11">
         <v>71</v>
@@ -14008,7 +13995,7 @@
         <v>10</v>
       </c>
       <c r="J495" s="11">
-        <v>11.43</v>
+        <v>5.48</v>
       </c>
     </row>
     <row r="496" spans="1:10" x14ac:dyDescent="0.25">
@@ -14021,8 +14008,8 @@
       <c r="C496" s="8">
         <v>45867</v>
       </c>
-      <c r="D496" s="16">
-        <v>86</v>
+      <c r="D496">
+        <v>75</v>
       </c>
       <c r="E496" s="11">
         <v>73.5</v>
@@ -14037,7 +14024,7 @@
         <v>9</v>
       </c>
       <c r="J496" s="11">
-        <v>10.72</v>
+        <v>13.51</v>
       </c>
     </row>
     <row r="497" spans="1:10" x14ac:dyDescent="0.25">
@@ -14050,8 +14037,8 @@
       <c r="C497" s="8">
         <v>45868</v>
       </c>
-      <c r="D497" s="16">
-        <v>137</v>
+      <c r="D497">
+        <v>139</v>
       </c>
       <c r="E497" s="11">
         <v>73</v>
@@ -14066,7 +14053,7 @@
         <v>8</v>
       </c>
       <c r="J497" s="11">
-        <v>12.93</v>
+        <v>9.5500000000000007</v>
       </c>
     </row>
     <row r="498" spans="1:10" x14ac:dyDescent="0.25">
@@ -14079,8 +14066,8 @@
       <c r="C498" s="8">
         <v>45869</v>
       </c>
-      <c r="D498" s="16">
-        <v>169</v>
+      <c r="D498">
+        <v>159</v>
       </c>
       <c r="E498" s="11">
         <v>70</v>
@@ -14095,7 +14082,7 @@
         <v>9</v>
       </c>
       <c r="J498" s="11">
-        <v>7.75</v>
+        <v>7.45</v>
       </c>
     </row>
     <row r="499" spans="1:10" x14ac:dyDescent="0.25">
@@ -14108,8 +14095,8 @@
       <c r="C499" s="8">
         <v>45870</v>
       </c>
-      <c r="D499" s="16">
-        <v>175</v>
+      <c r="D499">
+        <v>172</v>
       </c>
       <c r="E499" s="11">
         <v>70</v>
@@ -14124,7 +14111,7 @@
         <v>8</v>
       </c>
       <c r="J499" s="11">
-        <v>8.0299999999999994</v>
+        <v>6.05</v>
       </c>
     </row>
     <row r="500" spans="1:10" x14ac:dyDescent="0.25">
@@ -14137,8 +14124,8 @@
       <c r="C500" s="8">
         <v>45871</v>
       </c>
-      <c r="D500" s="16">
-        <v>51</v>
+      <c r="D500">
+        <v>54</v>
       </c>
       <c r="E500" s="11">
         <v>69</v>
@@ -14153,7 +14140,7 @@
         <v>4</v>
       </c>
       <c r="J500" s="11">
-        <v>12.99</v>
+        <v>9.56</v>
       </c>
     </row>
     <row r="501" spans="1:10" x14ac:dyDescent="0.25">
@@ -14166,8 +14153,8 @@
       <c r="C501" s="8">
         <v>45872</v>
       </c>
-      <c r="D501" s="16">
-        <v>64</v>
+      <c r="D501">
+        <v>59</v>
       </c>
       <c r="E501" s="11">
         <v>71</v>
@@ -14182,7 +14169,7 @@
         <v>6</v>
       </c>
       <c r="J501" s="11">
-        <v>9.0299999999999994</v>
+        <v>5.14</v>
       </c>
     </row>
     <row r="502" spans="1:10" x14ac:dyDescent="0.25">
@@ -14195,8 +14182,8 @@
       <c r="C502" s="8">
         <v>45873</v>
       </c>
-      <c r="D502" s="16">
-        <v>68</v>
+      <c r="D502">
+        <v>70</v>
       </c>
       <c r="E502" s="11">
         <v>74.5</v>
@@ -14211,7 +14198,7 @@
         <v>5</v>
       </c>
       <c r="J502" s="11">
-        <v>7.32</v>
+        <v>10.42</v>
       </c>
     </row>
     <row r="503" spans="1:10" x14ac:dyDescent="0.25">
@@ -14224,8 +14211,8 @@
       <c r="C503" s="8">
         <v>45874</v>
       </c>
-      <c r="D503" s="16">
-        <v>54</v>
+      <c r="D503">
+        <v>60</v>
       </c>
       <c r="E503" s="11">
         <v>73.5</v>
@@ -14240,7 +14227,7 @@
         <v>5</v>
       </c>
       <c r="J503" s="11">
-        <v>6.71</v>
+        <v>5.62</v>
       </c>
     </row>
     <row r="504" spans="1:10" x14ac:dyDescent="0.25">
@@ -14253,8 +14240,8 @@
       <c r="C504" s="8">
         <v>45875</v>
       </c>
-      <c r="D504" s="16">
-        <v>117</v>
+      <c r="D504">
+        <v>107</v>
       </c>
       <c r="E504" s="11">
         <v>69</v>
@@ -14269,7 +14256,7 @@
         <v>9</v>
       </c>
       <c r="J504" s="11">
-        <v>9.6300000000000008</v>
+        <v>7.81</v>
       </c>
     </row>
     <row r="505" spans="1:10" x14ac:dyDescent="0.25">
@@ -14282,8 +14269,8 @@
       <c r="C505" s="8">
         <v>45876</v>
       </c>
-      <c r="D505" s="16">
-        <v>140</v>
+      <c r="D505">
+        <v>124</v>
       </c>
       <c r="E505" s="11">
         <v>68.5</v>
@@ -14298,7 +14285,7 @@
         <v>5</v>
       </c>
       <c r="J505" s="11">
-        <v>13.69</v>
+        <v>7.86</v>
       </c>
     </row>
     <row r="506" spans="1:10" x14ac:dyDescent="0.25">
@@ -14311,8 +14298,8 @@
       <c r="C506" s="8">
         <v>45877</v>
       </c>
-      <c r="D506" s="16">
-        <v>186</v>
+      <c r="D506">
+        <v>181</v>
       </c>
       <c r="E506" s="11">
         <v>69.5</v>
@@ -14327,7 +14314,7 @@
         <v>6</v>
       </c>
       <c r="J506" s="11">
-        <v>5.96</v>
+        <v>5.92</v>
       </c>
     </row>
     <row r="507" spans="1:10" x14ac:dyDescent="0.25">
@@ -14340,8 +14327,8 @@
       <c r="C507" s="8">
         <v>45878</v>
       </c>
-      <c r="D507" s="16">
-        <v>57</v>
+      <c r="D507">
+        <v>66</v>
       </c>
       <c r="E507" s="11">
         <v>72</v>
@@ -14356,7 +14343,7 @@
         <v>15</v>
       </c>
       <c r="J507" s="11">
-        <v>11.7</v>
+        <v>8.73</v>
       </c>
     </row>
     <row r="508" spans="1:10" x14ac:dyDescent="0.25">
@@ -14369,8 +14356,8 @@
       <c r="C508" s="8">
         <v>45879</v>
       </c>
-      <c r="D508" s="16">
-        <v>58</v>
+      <c r="D508">
+        <v>62</v>
       </c>
       <c r="E508" s="11">
         <v>74.5</v>
@@ -14385,7 +14372,7 @@
         <v>12</v>
       </c>
       <c r="J508" s="11">
-        <v>8.42</v>
+        <v>10.63</v>
       </c>
     </row>
     <row r="509" spans="1:10" x14ac:dyDescent="0.25">
@@ -14398,8 +14385,8 @@
       <c r="C509" s="8">
         <v>45880</v>
       </c>
-      <c r="D509" s="16">
-        <v>60</v>
+      <c r="D509">
+        <v>58</v>
       </c>
       <c r="E509" s="11">
         <v>69.5</v>
@@ -14414,7 +14401,7 @@
         <v>8</v>
       </c>
       <c r="J509" s="11">
-        <v>10.36</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="510" spans="1:10" x14ac:dyDescent="0.25">
@@ -14427,8 +14414,8 @@
       <c r="C510" s="8">
         <v>45881</v>
       </c>
-      <c r="D510" s="16">
-        <v>63</v>
+      <c r="D510">
+        <v>65</v>
       </c>
       <c r="E510" s="11">
         <v>71.5</v>
@@ -14443,7 +14430,7 @@
         <v>5</v>
       </c>
       <c r="J510" s="11">
-        <v>6.76</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="511" spans="1:10" x14ac:dyDescent="0.25">
@@ -14456,8 +14443,8 @@
       <c r="C511" s="8">
         <v>45882</v>
       </c>
-      <c r="D511" s="16">
-        <v>81</v>
+      <c r="D511">
+        <v>77</v>
       </c>
       <c r="E511" s="11">
         <v>74</v>
@@ -14472,7 +14459,7 @@
         <v>5</v>
       </c>
       <c r="J511" s="11">
-        <v>6.96</v>
+        <v>5.41</v>
       </c>
     </row>
     <row r="512" spans="1:10" x14ac:dyDescent="0.25">
@@ -14499,8 +14486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8670AF5D-84FB-432F-8F14-677D63D19C50}">
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3:R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14604,7 +14591,7 @@
         <v>-45</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="S4:S18" si="3">O4/A4</f>
+        <f t="shared" ref="S4:S25" si="3">O4/A4</f>
         <v>0.71698113207547165</v>
       </c>
     </row>
@@ -14672,7 +14659,7 @@
         <v>12.17</v>
       </c>
       <c r="R6" s="30">
-        <f t="shared" ref="R6:R18" si="4">O6-A6</f>
+        <f t="shared" ref="R6:R25" si="4">O6-A6</f>
         <v>9</v>
       </c>
       <c r="S6">
@@ -15149,7 +15136,9 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
+      <c r="A19" s="22">
+        <v>44</v>
+      </c>
       <c r="B19" s="26">
         <v>45844</v>
       </c>
@@ -15171,9 +15160,6 @@
       <c r="H19">
         <v>92</v>
       </c>
-      <c r="I19">
-        <v>67</v>
-      </c>
       <c r="J19">
         <v>97</v>
       </c>
@@ -15191,15 +15177,25 @@
       </c>
       <c r="O19" s="23">
         <f t="shared" si="0"/>
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P19" s="23">
         <f t="shared" si="1"/>
-        <v>10.14</v>
+        <v>8.7100000000000009</v>
+      </c>
+      <c r="R19" s="30">
+        <f t="shared" si="4"/>
+        <v>43</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="3"/>
+        <v>1.9772727272727273</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
+      <c r="A20" s="22">
+        <v>52</v>
+      </c>
       <c r="B20" s="26">
         <v>45845</v>
       </c>
@@ -15221,9 +15217,6 @@
       <c r="H20">
         <v>72</v>
       </c>
-      <c r="I20">
-        <v>83</v>
-      </c>
       <c r="J20">
         <v>80</v>
       </c>
@@ -15241,15 +15234,25 @@
       </c>
       <c r="O20" s="23">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P20" s="23">
         <f t="shared" si="1"/>
-        <v>18.559999999999999</v>
+        <v>18.75</v>
+      </c>
+      <c r="R20" s="30">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="3"/>
+        <v>1.25</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
+      <c r="A21" s="22">
+        <v>68</v>
+      </c>
       <c r="B21" s="26">
         <v>45846</v>
       </c>
@@ -15271,9 +15274,6 @@
       <c r="H21">
         <v>60</v>
       </c>
-      <c r="I21">
-        <v>68</v>
-      </c>
       <c r="J21">
         <v>68</v>
       </c>
@@ -15291,15 +15291,25 @@
       </c>
       <c r="O21" s="23">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P21" s="23">
         <f t="shared" si="1"/>
-        <v>6.53</v>
+        <v>6.52</v>
+      </c>
+      <c r="R21" s="30">
+        <f t="shared" si="4"/>
+        <v>-6</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="3"/>
+        <v>0.91176470588235292</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
+      <c r="A22" s="22">
+        <v>64</v>
+      </c>
       <c r="B22" s="26">
         <v>45847</v>
       </c>
@@ -15321,9 +15331,6 @@
       <c r="H22">
         <v>95</v>
       </c>
-      <c r="I22">
-        <v>101</v>
-      </c>
       <c r="J22">
         <v>104</v>
       </c>
@@ -15341,15 +15348,25 @@
       </c>
       <c r="O22" s="23">
         <f t="shared" si="0"/>
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P22" s="23">
         <f t="shared" si="1"/>
-        <v>17.97</v>
+        <v>18.239999999999998</v>
+      </c>
+      <c r="R22" s="30">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="3"/>
+        <v>1.328125</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
+      <c r="A23" s="22">
+        <v>85</v>
+      </c>
       <c r="B23" s="26">
         <v>45848</v>
       </c>
@@ -15371,9 +15388,6 @@
       <c r="H23">
         <v>110</v>
       </c>
-      <c r="I23">
-        <v>153</v>
-      </c>
       <c r="J23">
         <v>137</v>
       </c>
@@ -15391,111 +15405,139 @@
       </c>
       <c r="O23" s="23">
         <f t="shared" si="0"/>
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="P23" s="23">
         <f t="shared" si="1"/>
-        <v>22.01</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="26">
+        <v>20.82</v>
+      </c>
+      <c r="R23" s="30">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="3"/>
+        <v>1.3529411764705883</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="34">
+        <v>146</v>
+      </c>
+      <c r="B24" s="35">
         <v>45849</v>
       </c>
-      <c r="C24" s="18">
-        <v>179</v>
-      </c>
-      <c r="D24">
+      <c r="C24" s="36">
+        <v>135</v>
+      </c>
+      <c r="D24" s="37">
+        <v>195</v>
+      </c>
+      <c r="E24" s="37">
+        <v>134</v>
+      </c>
+      <c r="F24" s="37">
+        <v>193</v>
+      </c>
+      <c r="G24" s="37">
+        <v>204</v>
+      </c>
+      <c r="H24" s="37">
+        <v>176</v>
+      </c>
+      <c r="I24" s="37">
+        <v>180</v>
+      </c>
+      <c r="J24" s="37">
+        <v>219</v>
+      </c>
+      <c r="K24" s="37">
+        <v>144</v>
+      </c>
+      <c r="L24" s="37">
+        <v>192</v>
+      </c>
+      <c r="M24" s="37">
+        <v>128</v>
+      </c>
+      <c r="N24" s="37">
+        <v>214</v>
+      </c>
+      <c r="O24" s="38">
+        <f t="shared" si="0"/>
+        <v>176</v>
+      </c>
+      <c r="P24" s="38">
+        <f t="shared" si="1"/>
+        <v>28.78</v>
+      </c>
+      <c r="R24" s="39">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="S24" s="37">
+        <f t="shared" si="3"/>
+        <v>1.2054794520547945</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="22">
         <v>178</v>
       </c>
-      <c r="E24">
-        <v>209</v>
-      </c>
-      <c r="F24">
-        <v>152</v>
-      </c>
-      <c r="G24">
-        <v>178</v>
-      </c>
-      <c r="H24">
-        <v>208</v>
-      </c>
-      <c r="I24">
-        <v>202</v>
-      </c>
-      <c r="J24">
-        <v>229</v>
-      </c>
-      <c r="K24">
-        <v>174</v>
-      </c>
-      <c r="L24">
-        <v>206</v>
-      </c>
-      <c r="M24">
-        <v>192</v>
-      </c>
-      <c r="N24">
-        <v>171</v>
-      </c>
-      <c r="O24" s="23">
-        <f t="shared" si="0"/>
-        <v>190</v>
-      </c>
-      <c r="P24" s="23">
-        <f t="shared" si="1"/>
-        <v>20.309999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
       <c r="B25" s="26">
         <v>45850</v>
       </c>
       <c r="C25" s="18">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D25">
+        <v>174</v>
+      </c>
+      <c r="E25">
+        <v>175</v>
+      </c>
+      <c r="F25">
+        <v>158</v>
+      </c>
+      <c r="G25">
+        <v>172</v>
+      </c>
+      <c r="H25">
+        <v>159</v>
+      </c>
+      <c r="I25">
+        <v>169</v>
+      </c>
+      <c r="J25">
+        <v>183</v>
+      </c>
+      <c r="K25">
+        <v>173</v>
+      </c>
+      <c r="L25">
+        <v>182</v>
+      </c>
+      <c r="M25">
+        <v>151</v>
+      </c>
+      <c r="N25">
         <v>165</v>
-      </c>
-      <c r="E25">
-        <v>166</v>
-      </c>
-      <c r="F25">
-        <v>162</v>
-      </c>
-      <c r="G25">
-        <v>162</v>
-      </c>
-      <c r="H25">
-        <v>157</v>
-      </c>
-      <c r="I25">
-        <v>161</v>
-      </c>
-      <c r="J25">
-        <v>163</v>
-      </c>
-      <c r="K25">
-        <v>162</v>
-      </c>
-      <c r="L25">
-        <v>158</v>
-      </c>
-      <c r="M25">
-        <v>170</v>
-      </c>
-      <c r="N25">
-        <v>158</v>
       </c>
       <c r="O25" s="23">
         <f t="shared" si="0"/>
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="P25" s="23">
         <f t="shared" si="1"/>
-        <v>3.51</v>
+        <v>9.18</v>
+      </c>
+      <c r="R25" s="39">
+        <f t="shared" si="4"/>
+        <v>-9</v>
+      </c>
+      <c r="S25" s="37">
+        <f t="shared" si="3"/>
+        <v>0.949438202247191</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -15504,48 +15546,48 @@
         <v>45851</v>
       </c>
       <c r="C26" s="18">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="D26">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="E26">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="F26">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="G26">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="H26">
         <v>79</v>
       </c>
       <c r="I26">
+        <v>86</v>
+      </c>
+      <c r="J26">
+        <v>70</v>
+      </c>
+      <c r="K26">
+        <v>79</v>
+      </c>
+      <c r="L26">
+        <v>78</v>
+      </c>
+      <c r="M26">
         <v>84</v>
       </c>
-      <c r="J26">
-        <v>77</v>
-      </c>
-      <c r="K26">
-        <v>57</v>
-      </c>
-      <c r="L26">
-        <v>68</v>
-      </c>
-      <c r="M26">
-        <v>72</v>
-      </c>
       <c r="N26">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="O26" s="23">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="P26" s="23">
         <f t="shared" si="1"/>
-        <v>11.91</v>
+        <v>5.58</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -15554,48 +15596,48 @@
         <v>45852</v>
       </c>
       <c r="C27" s="18">
+        <v>78</v>
+      </c>
+      <c r="D27">
         <v>85</v>
       </c>
-      <c r="D27">
-        <v>80</v>
-      </c>
       <c r="E27">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="F27">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G27">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H27">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I27">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="J27">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K27">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="L27">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="M27">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="N27">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="O27" s="23">
         <f t="shared" si="0"/>
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="P27" s="23">
         <f t="shared" si="1"/>
-        <v>10.48</v>
+        <v>5.59</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -15604,48 +15646,48 @@
         <v>45853</v>
       </c>
       <c r="C28" s="18">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D28">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="E28">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="F28">
         <v>78</v>
       </c>
       <c r="G28">
+        <v>85</v>
+      </c>
+      <c r="H28">
+        <v>72</v>
+      </c>
+      <c r="I28">
         <v>79</v>
       </c>
-      <c r="H28">
-        <v>81</v>
-      </c>
-      <c r="I28">
-        <v>76</v>
-      </c>
       <c r="J28">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="K28">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="L28">
+        <v>87</v>
+      </c>
+      <c r="M28">
+        <v>79</v>
+      </c>
+      <c r="N28">
         <v>86</v>
-      </c>
-      <c r="M28">
-        <v>91</v>
-      </c>
-      <c r="N28">
-        <v>73</v>
       </c>
       <c r="O28" s="23">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="P28" s="23">
         <f t="shared" si="1"/>
-        <v>8.67</v>
+        <v>4.3099999999999996</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -15654,40 +15696,40 @@
         <v>45854</v>
       </c>
       <c r="C29" s="18">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D29">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E29">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F29">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G29">
+        <v>89</v>
+      </c>
+      <c r="H29">
+        <v>86</v>
+      </c>
+      <c r="I29">
+        <v>83</v>
+      </c>
+      <c r="J29">
+        <v>92</v>
+      </c>
+      <c r="K29">
+        <v>68</v>
+      </c>
+      <c r="L29">
+        <v>86</v>
+      </c>
+      <c r="M29">
+        <v>78</v>
+      </c>
+      <c r="N29">
         <v>87</v>
-      </c>
-      <c r="H29">
-        <v>65</v>
-      </c>
-      <c r="I29">
-        <v>90</v>
-      </c>
-      <c r="J29">
-        <v>80</v>
-      </c>
-      <c r="K29">
-        <v>49</v>
-      </c>
-      <c r="L29">
-        <v>83</v>
-      </c>
-      <c r="M29">
-        <v>122</v>
-      </c>
-      <c r="N29">
-        <v>93</v>
       </c>
       <c r="O29" s="23">
         <f t="shared" si="0"/>
@@ -15695,7 +15737,7 @@
       </c>
       <c r="P29" s="23">
         <f t="shared" si="1"/>
-        <v>17.309999999999999</v>
+        <v>8.27</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -15704,48 +15746,48 @@
         <v>45855</v>
       </c>
       <c r="C30" s="18">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D30">
+        <v>100</v>
+      </c>
+      <c r="E30">
+        <v>114</v>
+      </c>
+      <c r="F30">
+        <v>90</v>
+      </c>
+      <c r="G30">
         <v>102</v>
       </c>
-      <c r="E30">
-        <v>61</v>
-      </c>
-      <c r="F30">
-        <v>96</v>
-      </c>
-      <c r="G30">
-        <v>89</v>
-      </c>
       <c r="H30">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="I30">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="J30">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="K30">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="L30">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="M30">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="N30">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="O30" s="23">
         <f t="shared" si="0"/>
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="P30" s="23">
         <f t="shared" si="1"/>
-        <v>13.07</v>
+        <v>9.44</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -15754,48 +15796,48 @@
         <v>45856</v>
       </c>
       <c r="C31" s="18">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D31">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="E31">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="F31">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="G31">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="H31">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="I31">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J31">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="K31">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="L31">
-        <v>119</v>
+        <v>154</v>
       </c>
       <c r="M31">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="N31">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="O31" s="23">
         <f t="shared" si="0"/>
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="P31" s="23">
         <f t="shared" si="1"/>
-        <v>7.64</v>
+        <v>14.37</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -15804,48 +15846,48 @@
         <v>45857</v>
       </c>
       <c r="C32" s="18">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D32">
+        <v>167</v>
+      </c>
+      <c r="E32">
+        <v>171</v>
+      </c>
+      <c r="F32">
+        <v>169</v>
+      </c>
+      <c r="G32">
+        <v>169</v>
+      </c>
+      <c r="H32">
+        <v>171</v>
+      </c>
+      <c r="I32">
+        <v>179</v>
+      </c>
+      <c r="J32">
+        <v>164</v>
+      </c>
+      <c r="K32">
         <v>176</v>
       </c>
-      <c r="E32">
-        <v>175</v>
-      </c>
-      <c r="F32">
+      <c r="L32">
+        <v>167</v>
+      </c>
+      <c r="M32">
+        <v>155</v>
+      </c>
+      <c r="N32">
         <v>170</v>
-      </c>
-      <c r="G32">
-        <v>172</v>
-      </c>
-      <c r="H32">
-        <v>172</v>
-      </c>
-      <c r="I32">
-        <v>168</v>
-      </c>
-      <c r="J32">
-        <v>168</v>
-      </c>
-      <c r="K32">
-        <v>165</v>
-      </c>
-      <c r="L32">
-        <v>168</v>
-      </c>
-      <c r="M32">
-        <v>165</v>
-      </c>
-      <c r="N32">
-        <v>161</v>
       </c>
       <c r="O32" s="23">
         <f t="shared" si="0"/>
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P32" s="23">
         <f t="shared" si="1"/>
-        <v>4.12</v>
+        <v>5.68</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -15854,48 +15896,48 @@
         <v>45858</v>
       </c>
       <c r="C33" s="18">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D33">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="E33">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F33">
         <v>45</v>
       </c>
       <c r="G33">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H33">
+        <v>57</v>
+      </c>
+      <c r="I33">
+        <v>48</v>
+      </c>
+      <c r="J33">
+        <v>45</v>
+      </c>
+      <c r="K33">
         <v>52</v>
       </c>
-      <c r="I33">
-        <v>37</v>
-      </c>
-      <c r="J33">
-        <v>49</v>
-      </c>
-      <c r="K33">
+      <c r="L33">
+        <v>54</v>
+      </c>
+      <c r="M33">
         <v>55</v>
       </c>
-      <c r="L33">
-        <v>49</v>
-      </c>
-      <c r="M33">
-        <v>41</v>
-      </c>
       <c r="N33">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="O33" s="23">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P33" s="23">
         <f t="shared" si="1"/>
-        <v>4.87</v>
+        <v>8.01</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -15904,48 +15946,48 @@
         <v>45859</v>
       </c>
       <c r="C34" s="18">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D34">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E34">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F34">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G34">
+        <v>62</v>
+      </c>
+      <c r="H34">
+        <v>62</v>
+      </c>
+      <c r="I34">
         <v>56</v>
       </c>
-      <c r="H34">
-        <v>60</v>
-      </c>
-      <c r="I34">
-        <v>66</v>
-      </c>
       <c r="J34">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="K34">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L34">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="M34">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="N34">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="O34" s="23">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P34" s="23">
         <f t="shared" si="1"/>
-        <v>4.46</v>
+        <v>5.28</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -15954,48 +15996,48 @@
         <v>45860</v>
       </c>
       <c r="C35" s="18">
+        <v>90</v>
+      </c>
+      <c r="D35">
+        <v>77</v>
+      </c>
+      <c r="E35">
+        <v>101</v>
+      </c>
+      <c r="F35">
         <v>81</v>
       </c>
-      <c r="D35">
+      <c r="G35">
         <v>92</v>
       </c>
-      <c r="E35">
-        <v>94</v>
-      </c>
-      <c r="F35">
-        <v>68</v>
-      </c>
-      <c r="G35">
-        <v>87</v>
-      </c>
       <c r="H35">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="I35">
+        <v>78</v>
+      </c>
+      <c r="J35">
+        <v>108</v>
+      </c>
+      <c r="K35">
+        <v>90</v>
+      </c>
+      <c r="L35">
+        <v>78</v>
+      </c>
+      <c r="M35">
+        <v>85</v>
+      </c>
+      <c r="N35">
         <v>103</v>
-      </c>
-      <c r="J35">
-        <v>101</v>
-      </c>
-      <c r="K35">
-        <v>99</v>
-      </c>
-      <c r="L35">
-        <v>110</v>
-      </c>
-      <c r="M35">
-        <v>102</v>
-      </c>
-      <c r="N35">
-        <v>88</v>
       </c>
       <c r="O35" s="23">
         <f t="shared" si="0"/>
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="P35" s="23">
         <f t="shared" si="1"/>
-        <v>12.34</v>
+        <v>12.95</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -16004,48 +16046,48 @@
         <v>45861</v>
       </c>
       <c r="C36" s="18">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="D36">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E36">
         <v>63</v>
       </c>
       <c r="F36">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G36">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="H36">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="I36">
         <v>66</v>
       </c>
       <c r="J36">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="K36">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="L36">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="M36">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="N36">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="O36" s="23">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="P36" s="23">
         <f t="shared" si="1"/>
-        <v>11.36</v>
+        <v>3.44</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -16054,48 +16096,48 @@
         <v>45862</v>
       </c>
       <c r="C37" s="18">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D37">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E37">
+        <v>72</v>
+      </c>
+      <c r="F37">
         <v>63</v>
       </c>
-      <c r="F37">
-        <v>95</v>
-      </c>
       <c r="G37">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H37">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I37">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J37">
         <v>80</v>
       </c>
       <c r="K37">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="L37">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="M37">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="N37">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="O37" s="23">
         <f t="shared" si="0"/>
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="P37" s="23">
         <f t="shared" si="1"/>
-        <v>8.2200000000000006</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -16104,48 +16146,48 @@
         <v>45863</v>
       </c>
       <c r="C38" s="18">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D38" s="18">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E38" s="18">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="F38" s="18">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="G38" s="18">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="H38" s="22">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="I38" s="18">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="J38" s="18">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="K38" s="18">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="L38" s="18">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="M38" s="18">
-        <v>180</v>
+        <v>154</v>
       </c>
       <c r="N38" s="19">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="O38" s="23">
         <f t="shared" ref="O38:O57" si="5">ROUND(AVERAGE(C38:N38),0)</f>
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="P38" s="23">
         <f>ROUND(_xlfn.STDEV.P(D38:O38),2)</f>
-        <v>10.050000000000001</v>
+        <v>14.57</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -16154,48 +16196,48 @@
         <v>45864</v>
       </c>
       <c r="C39" s="18">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="D39" s="18">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E39" s="18">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="F39" s="18">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="G39" s="18">
         <v>188</v>
       </c>
       <c r="H39" s="22">
+        <v>168</v>
+      </c>
+      <c r="I39" s="18">
+        <v>191</v>
+      </c>
+      <c r="J39" s="18">
+        <v>197</v>
+      </c>
+      <c r="K39" s="18">
         <v>185</v>
       </c>
-      <c r="I39" s="18">
-        <v>186</v>
-      </c>
-      <c r="J39" s="18">
-        <v>181</v>
-      </c>
-      <c r="K39" s="18">
-        <v>187</v>
-      </c>
       <c r="L39" s="18">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="M39" s="18">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="N39" s="19">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="O39" s="23">
         <f t="shared" si="5"/>
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="P39" s="23">
         <f t="shared" ref="P39:P57" si="6">ROUND(_xlfn.STDEV.P(D39:O39),2)</f>
-        <v>3.65</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -16204,48 +16246,48 @@
         <v>45865</v>
       </c>
       <c r="C40" s="18">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D40" s="18">
+        <v>58</v>
+      </c>
+      <c r="E40" s="18">
+        <v>65</v>
+      </c>
+      <c r="F40" s="18">
+        <v>59</v>
+      </c>
+      <c r="G40" s="18">
         <v>68</v>
       </c>
-      <c r="E40" s="18">
-        <v>63</v>
-      </c>
-      <c r="F40" s="18">
-        <v>52</v>
-      </c>
-      <c r="G40" s="18">
-        <v>67</v>
-      </c>
       <c r="H40" s="22">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I40" s="18">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="J40" s="18">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="K40" s="18">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="L40" s="18">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="M40" s="18">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="N40" s="19">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="O40" s="23">
         <f t="shared" si="5"/>
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="P40" s="23">
         <f t="shared" si="6"/>
-        <v>11.37</v>
+        <v>4.74</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -16254,48 +16296,48 @@
         <v>45866</v>
       </c>
       <c r="C41" s="18">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D41" s="18">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E41" s="18">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F41" s="18">
+        <v>58</v>
+      </c>
+      <c r="G41" s="18">
         <v>67</v>
       </c>
-      <c r="G41" s="18">
-        <v>52</v>
-      </c>
       <c r="H41" s="22">
+        <v>63</v>
+      </c>
+      <c r="I41" s="18">
+        <v>61</v>
+      </c>
+      <c r="J41" s="18">
+        <v>50</v>
+      </c>
+      <c r="K41" s="18">
+        <v>63</v>
+      </c>
+      <c r="L41" s="18">
+        <v>53</v>
+      </c>
+      <c r="M41" s="18">
         <v>62</v>
       </c>
-      <c r="I41" s="18">
-        <v>65</v>
-      </c>
-      <c r="J41" s="18">
-        <v>67</v>
-      </c>
-      <c r="K41" s="18">
-        <v>71</v>
-      </c>
-      <c r="L41" s="18">
-        <v>83</v>
-      </c>
-      <c r="M41" s="18">
-        <v>33</v>
-      </c>
       <c r="N41" s="19">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="O41" s="23">
         <f t="shared" si="5"/>
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="P41" s="23">
         <f t="shared" si="6"/>
-        <v>11.43</v>
+        <v>5.48</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -16304,48 +16346,48 @@
         <v>45867</v>
       </c>
       <c r="C42" s="18">
-        <v>130</v>
+        <v>81</v>
       </c>
       <c r="D42" s="18">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="E42" s="18">
+        <v>82</v>
+      </c>
+      <c r="F42" s="18">
+        <v>52</v>
+      </c>
+      <c r="G42" s="18">
+        <v>78</v>
+      </c>
+      <c r="H42" s="22">
+        <v>99</v>
+      </c>
+      <c r="I42" s="18">
+        <v>70</v>
+      </c>
+      <c r="J42" s="18">
+        <v>51</v>
+      </c>
+      <c r="K42" s="18">
+        <v>77</v>
+      </c>
+      <c r="L42" s="18">
         <v>88</v>
       </c>
-      <c r="F42" s="18">
-        <v>80</v>
-      </c>
-      <c r="G42" s="18">
-        <v>84</v>
-      </c>
-      <c r="H42" s="22">
-        <v>94</v>
-      </c>
-      <c r="I42" s="18">
-        <v>76</v>
-      </c>
-      <c r="J42" s="18">
-        <v>74</v>
-      </c>
-      <c r="K42" s="18">
-        <v>98</v>
-      </c>
-      <c r="L42" s="18">
-        <v>69</v>
-      </c>
       <c r="M42" s="18">
+        <v>68</v>
+      </c>
+      <c r="N42" s="19">
         <v>87</v>
-      </c>
-      <c r="N42" s="19">
-        <v>58</v>
       </c>
       <c r="O42" s="23">
         <f t="shared" si="5"/>
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="P42" s="23">
         <f t="shared" si="6"/>
-        <v>10.72</v>
+        <v>13.51</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -16354,48 +16396,48 @@
         <v>45868</v>
       </c>
       <c r="C43" s="18">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="D43" s="18">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="E43" s="18">
+        <v>139</v>
+      </c>
+      <c r="F43" s="18">
+        <v>144</v>
+      </c>
+      <c r="G43" s="18">
+        <v>140</v>
+      </c>
+      <c r="H43" s="22">
+        <v>115</v>
+      </c>
+      <c r="I43" s="18">
+        <v>159</v>
+      </c>
+      <c r="J43" s="18">
+        <v>136</v>
+      </c>
+      <c r="K43" s="18">
+        <v>137</v>
+      </c>
+      <c r="L43" s="18">
+        <v>141</v>
+      </c>
+      <c r="M43" s="18">
+        <v>134</v>
+      </c>
+      <c r="N43" s="19">
         <v>145</v>
-      </c>
-      <c r="F43" s="18">
-        <v>104</v>
-      </c>
-      <c r="G43" s="18">
-        <v>144</v>
-      </c>
-      <c r="H43" s="22">
-        <v>145</v>
-      </c>
-      <c r="I43" s="18">
-        <v>131</v>
-      </c>
-      <c r="J43" s="18">
-        <v>139</v>
-      </c>
-      <c r="K43" s="18">
-        <v>121</v>
-      </c>
-      <c r="L43" s="18">
-        <v>148</v>
-      </c>
-      <c r="M43" s="18">
-        <v>151</v>
-      </c>
-      <c r="N43" s="19">
-        <v>125</v>
       </c>
       <c r="O43" s="23">
         <f t="shared" si="5"/>
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="P43" s="23">
         <f t="shared" si="6"/>
-        <v>12.93</v>
+        <v>9.5500000000000007</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -16404,48 +16446,48 @@
         <v>45869</v>
       </c>
       <c r="C44" s="18">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="D44" s="18">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="E44" s="18">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F44" s="18">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="G44" s="18">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="H44" s="22">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="I44" s="18">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="J44" s="18">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="K44" s="18">
         <v>166</v>
       </c>
       <c r="L44" s="18">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="M44" s="18">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="N44" s="19">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="O44" s="23">
         <f t="shared" si="5"/>
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="P44" s="23">
         <f t="shared" si="6"/>
-        <v>7.75</v>
+        <v>7.45</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -16454,48 +16496,48 @@
         <v>45870</v>
       </c>
       <c r="C45" s="18">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="D45" s="18">
+        <v>164</v>
+      </c>
+      <c r="E45" s="18">
+        <v>174</v>
+      </c>
+      <c r="F45" s="18">
+        <v>174</v>
+      </c>
+      <c r="G45" s="18">
         <v>173</v>
       </c>
-      <c r="E45" s="18">
-        <v>179</v>
-      </c>
-      <c r="F45" s="18">
-        <v>183</v>
-      </c>
-      <c r="G45" s="18">
-        <v>171</v>
-      </c>
       <c r="H45" s="22">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="I45" s="18">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="J45" s="18">
-        <v>189</v>
+        <v>157</v>
       </c>
       <c r="K45" s="18">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="L45" s="18">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="M45" s="18">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="N45" s="19">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="O45" s="23">
         <f t="shared" si="5"/>
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="P45" s="23">
         <f t="shared" si="6"/>
-        <v>8.0299999999999994</v>
+        <v>6.05</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -16504,48 +16546,48 @@
         <v>45871</v>
       </c>
       <c r="C46" s="18">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D46" s="18">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E46" s="18">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F46" s="18">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G46" s="18">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="H46" s="22">
+        <v>63</v>
+      </c>
+      <c r="I46" s="18">
+        <v>66</v>
+      </c>
+      <c r="J46" s="18">
         <v>55</v>
       </c>
-      <c r="I46" s="18">
-        <v>29</v>
-      </c>
-      <c r="J46" s="18">
+      <c r="K46" s="18">
         <v>57</v>
-      </c>
-      <c r="K46" s="18">
-        <v>52</v>
       </c>
       <c r="L46" s="18">
         <v>63</v>
       </c>
       <c r="M46" s="18">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="N46" s="19">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="O46" s="23">
         <f t="shared" si="5"/>
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="P46" s="23">
         <f t="shared" si="6"/>
-        <v>12.99</v>
+        <v>9.56</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -16557,45 +16599,45 @@
         <v>69</v>
       </c>
       <c r="D47" s="18">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="E47" s="18">
         <v>60</v>
       </c>
       <c r="F47" s="18">
+        <v>53</v>
+      </c>
+      <c r="G47" s="18">
+        <v>58</v>
+      </c>
+      <c r="H47" s="22">
+        <v>54</v>
+      </c>
+      <c r="I47" s="18">
+        <v>46</v>
+      </c>
+      <c r="J47" s="18">
+        <v>68</v>
+      </c>
+      <c r="K47" s="18">
+        <v>62</v>
+      </c>
+      <c r="L47" s="18">
+        <v>59</v>
+      </c>
+      <c r="M47" s="18">
+        <v>58</v>
+      </c>
+      <c r="N47" s="19">
         <v>61</v>
-      </c>
-      <c r="G47" s="18">
-        <v>72</v>
-      </c>
-      <c r="H47" s="22">
-        <v>58</v>
-      </c>
-      <c r="I47" s="18">
-        <v>73</v>
-      </c>
-      <c r="J47" s="18">
-        <v>50</v>
-      </c>
-      <c r="K47" s="18">
-        <v>71</v>
-      </c>
-      <c r="L47" s="18">
-        <v>56</v>
-      </c>
-      <c r="M47" s="18">
-        <v>51</v>
-      </c>
-      <c r="N47" s="19">
-        <v>60</v>
       </c>
       <c r="O47" s="23">
         <f t="shared" si="5"/>
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="P47" s="23">
         <f t="shared" si="6"/>
-        <v>9.0299999999999994</v>
+        <v>5.14</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -16607,45 +16649,45 @@
         <v>75</v>
       </c>
       <c r="D48" s="18">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="E48" s="18">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F48" s="18">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="G48" s="18">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="H48" s="22">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I48" s="18">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J48" s="18">
         <v>62</v>
       </c>
       <c r="K48" s="18">
+        <v>69</v>
+      </c>
+      <c r="L48" s="18">
         <v>71</v>
       </c>
-      <c r="L48" s="18">
+      <c r="M48" s="18">
         <v>63</v>
       </c>
-      <c r="M48" s="18">
-        <v>69</v>
-      </c>
       <c r="N48" s="19">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="O48" s="23">
         <f t="shared" si="5"/>
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="P48" s="23">
         <f t="shared" si="6"/>
-        <v>7.32</v>
+        <v>10.42</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -16654,48 +16696,48 @@
         <v>45874</v>
       </c>
       <c r="C49" s="18">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D49" s="18">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E49" s="18">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F49" s="18">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G49" s="18">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="H49" s="22">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="I49" s="18">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="J49" s="18">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="K49" s="18">
         <v>59</v>
       </c>
       <c r="L49" s="18">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="M49" s="18">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N49" s="19">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="O49" s="23">
         <f t="shared" si="5"/>
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="P49" s="23">
         <f t="shared" si="6"/>
-        <v>6.71</v>
+        <v>5.62</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -16704,48 +16746,48 @@
         <v>45875</v>
       </c>
       <c r="C50" s="18">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="D50" s="18">
+        <v>110</v>
+      </c>
+      <c r="E50" s="18">
+        <v>111</v>
+      </c>
+      <c r="F50" s="18">
+        <v>114</v>
+      </c>
+      <c r="G50" s="18">
+        <v>111</v>
+      </c>
+      <c r="H50" s="22">
         <v>115</v>
       </c>
-      <c r="E50" s="18">
-        <v>128</v>
-      </c>
-      <c r="F50" s="18">
+      <c r="I50" s="18">
+        <v>95</v>
+      </c>
+      <c r="J50" s="18">
+        <v>95</v>
+      </c>
+      <c r="K50" s="18">
+        <v>108</v>
+      </c>
+      <c r="L50" s="18">
+        <v>119</v>
+      </c>
+      <c r="M50" s="18">
         <v>98</v>
       </c>
-      <c r="G50" s="18">
-        <v>105</v>
-      </c>
-      <c r="H50" s="22">
-        <v>124</v>
-      </c>
-      <c r="I50" s="18">
-        <v>130</v>
-      </c>
-      <c r="J50" s="18">
-        <v>112</v>
-      </c>
-      <c r="K50" s="18">
-        <v>112</v>
-      </c>
-      <c r="L50" s="18">
-        <v>106</v>
-      </c>
-      <c r="M50" s="18">
-        <v>110</v>
-      </c>
       <c r="N50" s="19">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="O50" s="23">
         <f t="shared" si="5"/>
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="P50" s="23">
         <f t="shared" si="6"/>
-        <v>9.6300000000000008</v>
+        <v>7.81</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -16754,48 +16796,48 @@
         <v>45876</v>
       </c>
       <c r="C51" s="18">
-        <v>184</v>
+        <v>125</v>
       </c>
       <c r="D51" s="18">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="E51" s="18">
+        <v>124</v>
+      </c>
+      <c r="F51" s="18">
+        <v>119</v>
+      </c>
+      <c r="G51" s="18">
+        <v>129</v>
+      </c>
+      <c r="H51" s="22">
+        <v>116</v>
+      </c>
+      <c r="I51" s="18">
+        <v>133</v>
+      </c>
+      <c r="J51" s="18">
+        <v>123</v>
+      </c>
+      <c r="K51" s="18">
+        <v>139</v>
+      </c>
+      <c r="L51" s="18">
+        <v>118</v>
+      </c>
+      <c r="M51" s="18">
+        <v>108</v>
+      </c>
+      <c r="N51" s="19">
         <v>120</v>
-      </c>
-      <c r="F51" s="18">
-        <v>176</v>
-      </c>
-      <c r="G51" s="18">
-        <v>134</v>
-      </c>
-      <c r="H51" s="22">
-        <v>125</v>
-      </c>
-      <c r="I51" s="18">
-        <v>130</v>
-      </c>
-      <c r="J51" s="18">
-        <v>136</v>
-      </c>
-      <c r="K51" s="18">
-        <v>134</v>
-      </c>
-      <c r="L51" s="18">
-        <v>144</v>
-      </c>
-      <c r="M51" s="18">
-        <v>126</v>
-      </c>
-      <c r="N51" s="19">
-        <v>131</v>
       </c>
       <c r="O51" s="23">
         <f t="shared" si="5"/>
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="P51" s="23">
         <f t="shared" si="6"/>
-        <v>13.69</v>
+        <v>7.86</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -16804,48 +16846,48 @@
         <v>45877</v>
       </c>
       <c r="C52" s="18">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="D52" s="18">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E52" s="18">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="F52" s="18">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="G52" s="18">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H52" s="22">
         <v>174</v>
       </c>
       <c r="I52" s="18">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="J52" s="18">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="K52" s="18">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="L52" s="18">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="M52" s="18">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="N52" s="19">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="O52" s="23">
         <f t="shared" si="5"/>
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="P52" s="23">
         <f t="shared" si="6"/>
-        <v>5.96</v>
+        <v>5.92</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -16854,48 +16896,48 @@
         <v>45878</v>
       </c>
       <c r="C53" s="18">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D53" s="18">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E53" s="18">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F53" s="18">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="G53" s="18">
+        <v>59</v>
+      </c>
+      <c r="H53" s="22">
+        <v>77</v>
+      </c>
+      <c r="I53" s="18">
+        <v>48</v>
+      </c>
+      <c r="J53" s="18">
+        <v>77</v>
+      </c>
+      <c r="K53" s="18">
         <v>72</v>
       </c>
-      <c r="H53" s="22">
-        <v>62</v>
-      </c>
-      <c r="I53" s="18">
-        <v>56</v>
-      </c>
-      <c r="J53" s="18">
-        <v>58</v>
-      </c>
-      <c r="K53" s="18">
-        <v>49</v>
-      </c>
       <c r="L53" s="18">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="M53" s="18">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="N53" s="19">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="O53" s="23">
         <f t="shared" si="5"/>
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="P53" s="23">
         <f t="shared" si="6"/>
-        <v>11.7</v>
+        <v>8.73</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -16904,48 +16946,48 @@
         <v>45879</v>
       </c>
       <c r="C54" s="18">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D54" s="18">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E54" s="18">
+        <v>60</v>
+      </c>
+      <c r="F54" s="18">
+        <v>43</v>
+      </c>
+      <c r="G54" s="18">
+        <v>69</v>
+      </c>
+      <c r="H54" s="22">
+        <v>69</v>
+      </c>
+      <c r="I54" s="18">
+        <v>70</v>
+      </c>
+      <c r="J54" s="18">
+        <v>86</v>
+      </c>
+      <c r="K54" s="18">
+        <v>60</v>
+      </c>
+      <c r="L54" s="18">
         <v>59</v>
       </c>
-      <c r="F54" s="18">
-        <v>42</v>
-      </c>
-      <c r="G54" s="18">
-        <v>52</v>
-      </c>
-      <c r="H54" s="22">
-        <v>71</v>
-      </c>
-      <c r="I54" s="18">
-        <v>59</v>
-      </c>
-      <c r="J54" s="18">
-        <v>56</v>
-      </c>
-      <c r="K54" s="18">
-        <v>62</v>
-      </c>
-      <c r="L54" s="18">
-        <v>52</v>
-      </c>
       <c r="M54" s="18">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N54" s="19">
         <v>54</v>
       </c>
       <c r="O54" s="23">
         <f t="shared" si="5"/>
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="P54" s="23">
         <f t="shared" si="6"/>
-        <v>8.42</v>
+        <v>10.63</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -16954,48 +16996,48 @@
         <v>45880</v>
       </c>
       <c r="C55" s="18">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D55" s="18">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="E55" s="18">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F55" s="18">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="G55" s="18">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="H55" s="22">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I55" s="18">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="J55" s="18">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="K55" s="18">
         <v>55</v>
       </c>
       <c r="L55" s="18">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="M55" s="18">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N55" s="19">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="O55" s="23">
         <f t="shared" si="5"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P55" s="23">
         <f t="shared" si="6"/>
-        <v>10.36</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -17010,42 +17052,42 @@
         <v>61</v>
       </c>
       <c r="E56" s="18">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F56" s="18">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G56" s="18">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="H56" s="22">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I56" s="18">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J56" s="18">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K56" s="18">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="L56" s="18">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="M56" s="18">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="N56" s="19">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="O56" s="23">
         <f t="shared" si="5"/>
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="P56" s="23">
         <f t="shared" si="6"/>
-        <v>6.76</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="57" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17054,48 +17096,48 @@
         <v>45882</v>
       </c>
       <c r="C57" s="27">
+        <v>77</v>
+      </c>
+      <c r="D57" s="20">
+        <v>75</v>
+      </c>
+      <c r="E57" s="20">
+        <v>76</v>
+      </c>
+      <c r="F57" s="20">
+        <v>66</v>
+      </c>
+      <c r="G57" s="20">
+        <v>78</v>
+      </c>
+      <c r="H57" s="25">
         <v>81</v>
-      </c>
-      <c r="D57" s="20">
-        <v>83</v>
-      </c>
-      <c r="E57" s="20">
-        <v>69</v>
-      </c>
-      <c r="F57" s="20">
-        <v>99</v>
-      </c>
-      <c r="G57" s="20">
-        <v>80</v>
-      </c>
-      <c r="H57" s="25">
-        <v>80</v>
       </c>
       <c r="I57" s="20">
         <v>77</v>
       </c>
       <c r="J57" s="20">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="K57" s="20">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="L57" s="20">
         <v>84</v>
       </c>
       <c r="M57" s="20">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="N57" s="28">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="O57" s="24">
         <f t="shared" si="5"/>
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="P57" s="24">
         <f t="shared" si="6"/>
-        <v>6.96</v>
+        <v>5.41</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -17104,48 +17146,48 @@
         <v>40</v>
       </c>
       <c r="C58" s="18">
-        <v>28.99</v>
+        <v>27.99</v>
       </c>
       <c r="D58" s="18">
-        <v>33.33</v>
+        <v>25</v>
       </c>
       <c r="E58" s="18">
-        <v>31.88</v>
+        <v>25.1</v>
       </c>
       <c r="F58" s="18">
-        <v>27.54</v>
+        <v>23.61</v>
       </c>
       <c r="G58" s="18">
-        <v>29.58</v>
+        <v>23.38</v>
       </c>
       <c r="H58" s="22">
-        <v>26.76</v>
+        <v>23.61</v>
       </c>
       <c r="I58" s="18">
-        <v>25.35</v>
+        <v>23.61</v>
       </c>
       <c r="J58" s="18">
-        <v>25.35</v>
+        <v>25</v>
       </c>
       <c r="K58" s="18">
-        <v>28.57</v>
+        <v>23.51</v>
       </c>
       <c r="L58" s="18">
-        <v>26.76</v>
+        <v>23.61</v>
       </c>
       <c r="M58" s="18">
-        <v>25.35</v>
+        <v>26.39</v>
       </c>
       <c r="N58" s="19">
-        <v>27.14</v>
+        <v>29.17</v>
       </c>
       <c r="O58" s="23">
         <f>ROUND(AVERAGE(C58:N58),2)</f>
-        <v>28.05</v>
+        <v>25</v>
       </c>
       <c r="P58" s="23">
         <f>ROUND(_xlfn.STDEV.P(E58:O58),2)</f>
-        <v>1.91</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -17154,48 +17196,48 @@
         <v>41</v>
       </c>
       <c r="C59" s="18">
-        <v>31.5</v>
+        <v>29.61</v>
       </c>
       <c r="D59" s="18">
-        <v>28.97</v>
+        <v>34.6</v>
       </c>
       <c r="E59" s="18">
-        <v>27.38</v>
+        <v>26.46</v>
       </c>
       <c r="F59" s="18">
-        <v>35.72</v>
+        <v>29.1</v>
       </c>
       <c r="G59" s="18">
-        <v>31.32</v>
+        <v>32.94</v>
       </c>
       <c r="H59" s="22">
-        <v>34.130000000000003</v>
+        <v>28.69</v>
       </c>
       <c r="I59" s="18">
-        <v>30.58</v>
+        <v>30.29</v>
       </c>
       <c r="J59" s="18">
-        <v>27.72</v>
+        <v>34.450000000000003</v>
       </c>
       <c r="K59" s="18">
-        <v>25.8</v>
+        <v>29.16</v>
       </c>
       <c r="L59" s="18">
-        <v>25.62</v>
+        <v>34.89</v>
       </c>
       <c r="M59" s="18">
-        <v>31.59</v>
+        <v>28.78</v>
       </c>
       <c r="N59" s="18">
-        <v>23.54</v>
+        <v>29.39</v>
       </c>
       <c r="O59" s="23">
         <f>ROUND(AVERAGE(C59:N59),2)</f>
-        <v>29.49</v>
+        <v>30.7</v>
       </c>
       <c r="P59" s="23">
         <f>ROUND(_xlfn.STDEV.P(E59:O59),2)</f>
-        <v>3.58</v>
+        <v>2.4900000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -17215,12 +17257,15 @@
     <cfRule type="aboveAverage" dxfId="2" priority="2"/>
     <cfRule type="aboveAverage" dxfId="1" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3:R18">
+  <conditionalFormatting sqref="R3:R25">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="O25" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>